<commit_message>
last second thoughts in paper
</commit_message>
<xml_diff>
--- a/Report/Empirical Data.xlsx
+++ b/Report/Empirical Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kharp\Desktop\School\2024\S2024\CSCI2226-DatastructuresAndAlgorithms\SortingProject\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C855B24F-0B35-4854-A6D6-86B3FABAA886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3237D3DD-9C91-435E-A8FB-C488AD8973B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,7 +362,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -748,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,56 +837,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -896,6 +888,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -921,32 +922,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -14164,97 +14163,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="AY1" s="42" t="s">
+      <c r="AY1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="AZ1" s="45"/>
-      <c r="BA1" s="45"/>
-      <c r="BB1" s="45"/>
-      <c r="BC1" s="45"/>
-      <c r="BD1" s="43"/>
-      <c r="BE1" s="46" t="s">
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="46" t="s">
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" s="31"/>
+      <c r="BH1" s="35"/>
       <c r="BI1" s="47" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="42" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="42" t="s">
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="43"/>
-      <c r="AD2" s="42" t="s">
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="52"/>
+      <c r="AD2" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="42" t="s">
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AK2" s="45"/>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="45"/>
-      <c r="AN2" s="45"/>
-      <c r="AO2" s="43"/>
-      <c r="AP2" s="42" t="s">
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AQ2" s="45"/>
-      <c r="AR2" s="45"/>
-      <c r="AS2" s="45"/>
-      <c r="AT2" s="45"/>
-      <c r="AU2" s="43"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="52"/>
       <c r="AX2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AY2" s="40" t="s">
+      <c r="AY2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AZ2" s="41"/>
-      <c r="BA2" s="42" t="s">
+      <c r="AZ2" s="64"/>
+      <c r="BA2" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="BB2" s="43"/>
-      <c r="BC2" s="41" t="s">
+      <c r="BB2" s="52"/>
+      <c r="BC2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="BD2" s="44"/>
+      <c r="BD2" s="65"/>
       <c r="BE2" s="38"/>
-      <c r="BF2" s="35"/>
+      <c r="BF2" s="39"/>
       <c r="BG2" s="38"/>
-      <c r="BH2" s="35"/>
+      <c r="BH2" s="39"/>
       <c r="BI2" s="48"/>
     </row>
     <row r="3" spans="1:61" ht="17" thickBot="1" x14ac:dyDescent="0.4">
@@ -14396,38 +14395,38 @@
       <c r="AU3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AX3" s="46" t="s">
+      <c r="AX3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AY3" s="39" t="s">
+      <c r="AY3" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="AZ3" s="31"/>
-      <c r="BA3" s="36" t="s">
+      <c r="AZ3" s="35"/>
+      <c r="BA3" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BB3" s="31"/>
-      <c r="BC3" s="36" t="s">
+      <c r="BB3" s="35"/>
+      <c r="BC3" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BD3" s="31"/>
-      <c r="BE3" s="30" t="s">
+      <c r="BD3" s="35"/>
+      <c r="BE3" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BF3" s="31"/>
-      <c r="BG3" s="46" t="s">
+      <c r="BF3" s="35"/>
+      <c r="BG3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="BH3" s="31"/>
+      <c r="BH3" s="35"/>
       <c r="BI3" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="60" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="10">
@@ -14568,22 +14567,22 @@
         <f>AVERAGE(AP4:AT4)</f>
         <v>2.1795882600000001</v>
       </c>
-      <c r="AX4" s="37"/>
-      <c r="AY4" s="37"/>
-      <c r="AZ4" s="33"/>
-      <c r="BA4" s="37"/>
-      <c r="BB4" s="33"/>
-      <c r="BC4" s="37"/>
-      <c r="BD4" s="33"/>
-      <c r="BE4" s="32"/>
-      <c r="BF4" s="33"/>
-      <c r="BG4" s="37"/>
-      <c r="BH4" s="33"/>
+      <c r="AX4" s="36"/>
+      <c r="AY4" s="36"/>
+      <c r="AZ4" s="37"/>
+      <c r="BA4" s="36"/>
+      <c r="BB4" s="37"/>
+      <c r="BC4" s="36"/>
+      <c r="BD4" s="37"/>
+      <c r="BE4" s="67"/>
+      <c r="BF4" s="37"/>
+      <c r="BG4" s="36"/>
+      <c r="BH4" s="37"/>
       <c r="BI4" s="48"/>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A5" s="54"/>
-      <c r="B5" s="51"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="5">
         <v>100000</v>
       </c>
@@ -14726,22 +14725,22 @@
         <f t="shared" ref="AU5:AU39" si="5">AVERAGE(AP5:AT5)</f>
         <v>8.7173875799999987</v>
       </c>
-      <c r="AX5" s="37"/>
-      <c r="AY5" s="37"/>
-      <c r="AZ5" s="33"/>
-      <c r="BA5" s="37"/>
-      <c r="BB5" s="33"/>
-      <c r="BC5" s="37"/>
-      <c r="BD5" s="33"/>
-      <c r="BE5" s="32"/>
-      <c r="BF5" s="33"/>
-      <c r="BG5" s="37"/>
-      <c r="BH5" s="33"/>
+      <c r="AX5" s="36"/>
+      <c r="AY5" s="36"/>
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="36"/>
+      <c r="BB5" s="37"/>
+      <c r="BC5" s="36"/>
+      <c r="BD5" s="37"/>
+      <c r="BE5" s="67"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="36"/>
+      <c r="BH5" s="37"/>
       <c r="BI5" s="48"/>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A6" s="54"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="5">
         <v>175000</v>
       </c>
@@ -14884,22 +14883,22 @@
         <f t="shared" si="5"/>
         <v>26.446548279999995</v>
       </c>
-      <c r="AX6" s="37"/>
-      <c r="AY6" s="37"/>
-      <c r="AZ6" s="33"/>
-      <c r="BA6" s="37"/>
-      <c r="BB6" s="33"/>
-      <c r="BC6" s="37"/>
-      <c r="BD6" s="33"/>
-      <c r="BE6" s="32"/>
-      <c r="BF6" s="33"/>
-      <c r="BG6" s="37"/>
-      <c r="BH6" s="33"/>
+      <c r="AX6" s="36"/>
+      <c r="AY6" s="36"/>
+      <c r="AZ6" s="37"/>
+      <c r="BA6" s="36"/>
+      <c r="BB6" s="37"/>
+      <c r="BC6" s="36"/>
+      <c r="BD6" s="37"/>
+      <c r="BE6" s="67"/>
+      <c r="BF6" s="37"/>
+      <c r="BG6" s="36"/>
+      <c r="BH6" s="37"/>
       <c r="BI6" s="48"/>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A7" s="54"/>
-      <c r="B7" s="51"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="5">
         <v>300000</v>
       </c>
@@ -15042,22 +15041,22 @@
         <f t="shared" si="5"/>
         <v>81.228794319999992</v>
       </c>
-      <c r="AX7" s="37"/>
-      <c r="AY7" s="37"/>
-      <c r="AZ7" s="33"/>
-      <c r="BA7" s="37"/>
-      <c r="BB7" s="33"/>
-      <c r="BC7" s="37"/>
-      <c r="BD7" s="33"/>
-      <c r="BE7" s="32"/>
-      <c r="BF7" s="33"/>
-      <c r="BG7" s="37"/>
-      <c r="BH7" s="33"/>
+      <c r="AX7" s="36"/>
+      <c r="AY7" s="36"/>
+      <c r="AZ7" s="37"/>
+      <c r="BA7" s="36"/>
+      <c r="BB7" s="37"/>
+      <c r="BC7" s="36"/>
+      <c r="BD7" s="37"/>
+      <c r="BE7" s="67"/>
+      <c r="BF7" s="37"/>
+      <c r="BG7" s="36"/>
+      <c r="BH7" s="37"/>
       <c r="BI7" s="48"/>
     </row>
     <row r="8" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="54"/>
-      <c r="B8" s="51"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="5">
         <v>425000</v>
       </c>
@@ -15202,20 +15201,20 @@
       </c>
       <c r="AX8" s="38"/>
       <c r="AY8" s="38"/>
-      <c r="AZ8" s="35"/>
+      <c r="AZ8" s="39"/>
       <c r="BA8" s="38"/>
-      <c r="BB8" s="35"/>
+      <c r="BB8" s="39"/>
       <c r="BC8" s="38"/>
-      <c r="BD8" s="35"/>
-      <c r="BE8" s="34"/>
-      <c r="BF8" s="35"/>
+      <c r="BD8" s="39"/>
+      <c r="BE8" s="68"/>
+      <c r="BF8" s="39"/>
       <c r="BG8" s="38"/>
-      <c r="BH8" s="35"/>
+      <c r="BH8" s="39"/>
       <c r="BI8" s="49"/>
     </row>
     <row r="9" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="55"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="6">
         <v>550000</v>
       </c>
@@ -15358,38 +15357,38 @@
         <f t="shared" si="5"/>
         <v>262.80399759999995</v>
       </c>
-      <c r="AX9" s="37" t="s">
+      <c r="AX9" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="AY9" s="36" t="s">
+      <c r="AY9" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="AZ9" s="31"/>
-      <c r="BA9" s="36" t="s">
+      <c r="AZ9" s="35"/>
+      <c r="BA9" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BB9" s="31"/>
-      <c r="BC9" s="36" t="s">
+      <c r="BB9" s="35"/>
+      <c r="BC9" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BD9" s="31"/>
-      <c r="BE9" s="30" t="s">
+      <c r="BD9" s="35"/>
+      <c r="BE9" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BF9" s="31"/>
-      <c r="BG9" s="46" t="s">
+      <c r="BF9" s="35"/>
+      <c r="BG9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="BH9" s="31"/>
+      <c r="BH9" s="35"/>
       <c r="BI9" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="60" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="10">
@@ -15530,22 +15529,22 @@
         <f t="shared" si="5"/>
         <v>0.8840920000000001</v>
       </c>
-      <c r="AX10" s="37"/>
-      <c r="AY10" s="37"/>
-      <c r="AZ10" s="33"/>
-      <c r="BA10" s="37"/>
-      <c r="BB10" s="33"/>
-      <c r="BC10" s="37"/>
-      <c r="BD10" s="33"/>
-      <c r="BE10" s="32"/>
-      <c r="BF10" s="33"/>
-      <c r="BG10" s="37"/>
-      <c r="BH10" s="33"/>
+      <c r="AX10" s="36"/>
+      <c r="AY10" s="36"/>
+      <c r="AZ10" s="37"/>
+      <c r="BA10" s="36"/>
+      <c r="BB10" s="37"/>
+      <c r="BC10" s="36"/>
+      <c r="BD10" s="37"/>
+      <c r="BE10" s="67"/>
+      <c r="BF10" s="37"/>
+      <c r="BG10" s="36"/>
+      <c r="BH10" s="37"/>
       <c r="BI10" s="48"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="5">
         <v>100000</v>
       </c>
@@ -15688,22 +15687,22 @@
         <f t="shared" si="5"/>
         <v>3.5525640000000003</v>
       </c>
-      <c r="AX11" s="37"/>
-      <c r="AY11" s="37"/>
-      <c r="AZ11" s="33"/>
-      <c r="BA11" s="37"/>
-      <c r="BB11" s="33"/>
-      <c r="BC11" s="37"/>
-      <c r="BD11" s="33"/>
-      <c r="BE11" s="32"/>
-      <c r="BF11" s="33"/>
-      <c r="BG11" s="37"/>
-      <c r="BH11" s="33"/>
+      <c r="AX11" s="36"/>
+      <c r="AY11" s="36"/>
+      <c r="AZ11" s="37"/>
+      <c r="BA11" s="36"/>
+      <c r="BB11" s="37"/>
+      <c r="BC11" s="36"/>
+      <c r="BD11" s="37"/>
+      <c r="BE11" s="67"/>
+      <c r="BF11" s="37"/>
+      <c r="BG11" s="36"/>
+      <c r="BH11" s="37"/>
       <c r="BI11" s="48"/>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A12" s="54"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="5">
         <v>175000</v>
       </c>
@@ -15846,22 +15845,22 @@
         <f t="shared" si="5"/>
         <v>10.935985580000001</v>
       </c>
-      <c r="AX12" s="37"/>
-      <c r="AY12" s="37"/>
-      <c r="AZ12" s="33"/>
-      <c r="BA12" s="37"/>
-      <c r="BB12" s="33"/>
-      <c r="BC12" s="37"/>
-      <c r="BD12" s="33"/>
-      <c r="BE12" s="32"/>
-      <c r="BF12" s="33"/>
-      <c r="BG12" s="37"/>
-      <c r="BH12" s="33"/>
+      <c r="AX12" s="36"/>
+      <c r="AY12" s="36"/>
+      <c r="AZ12" s="37"/>
+      <c r="BA12" s="36"/>
+      <c r="BB12" s="37"/>
+      <c r="BC12" s="36"/>
+      <c r="BD12" s="37"/>
+      <c r="BE12" s="67"/>
+      <c r="BF12" s="37"/>
+      <c r="BG12" s="36"/>
+      <c r="BH12" s="37"/>
       <c r="BI12" s="48"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A13" s="54"/>
-      <c r="B13" s="51"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="5">
         <v>300000</v>
       </c>
@@ -16004,22 +16003,22 @@
         <f t="shared" si="5"/>
         <v>32.4724115</v>
       </c>
-      <c r="AX13" s="37"/>
-      <c r="AY13" s="37"/>
-      <c r="AZ13" s="33"/>
-      <c r="BA13" s="37"/>
-      <c r="BB13" s="33"/>
-      <c r="BC13" s="37"/>
-      <c r="BD13" s="33"/>
-      <c r="BE13" s="32"/>
-      <c r="BF13" s="33"/>
-      <c r="BG13" s="37"/>
-      <c r="BH13" s="33"/>
+      <c r="AX13" s="36"/>
+      <c r="AY13" s="36"/>
+      <c r="AZ13" s="37"/>
+      <c r="BA13" s="36"/>
+      <c r="BB13" s="37"/>
+      <c r="BC13" s="36"/>
+      <c r="BD13" s="37"/>
+      <c r="BE13" s="67"/>
+      <c r="BF13" s="37"/>
+      <c r="BG13" s="36"/>
+      <c r="BH13" s="37"/>
       <c r="BI13" s="48"/>
     </row>
     <row r="14" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="5">
         <v>425000</v>
       </c>
@@ -16164,20 +16163,20 @@
       </c>
       <c r="AX14" s="38"/>
       <c r="AY14" s="38"/>
-      <c r="AZ14" s="35"/>
+      <c r="AZ14" s="39"/>
       <c r="BA14" s="38"/>
-      <c r="BB14" s="35"/>
+      <c r="BB14" s="39"/>
       <c r="BC14" s="38"/>
-      <c r="BD14" s="35"/>
-      <c r="BE14" s="34"/>
-      <c r="BF14" s="35"/>
+      <c r="BD14" s="39"/>
+      <c r="BE14" s="68"/>
+      <c r="BF14" s="39"/>
       <c r="BG14" s="38"/>
-      <c r="BH14" s="35"/>
+      <c r="BH14" s="39"/>
       <c r="BI14" s="49"/>
     </row>
     <row r="15" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="55"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="6">
         <v>550000</v>
       </c>
@@ -16320,38 +16319,38 @@
         <f t="shared" si="5"/>
         <v>110.83381118</v>
       </c>
-      <c r="AX15" s="46" t="s">
+      <c r="AX15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AY15" s="36" t="s">
+      <c r="AY15" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="AZ15" s="31"/>
-      <c r="BA15" s="36" t="s">
+      <c r="AZ15" s="35"/>
+      <c r="BA15" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BB15" s="31"/>
-      <c r="BC15" s="36" t="s">
+      <c r="BB15" s="35"/>
+      <c r="BC15" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BD15" s="31"/>
-      <c r="BE15" s="30" t="s">
+      <c r="BD15" s="35"/>
+      <c r="BE15" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BF15" s="31"/>
-      <c r="BG15" s="46" t="s">
+      <c r="BF15" s="35"/>
+      <c r="BG15" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="BH15" s="31"/>
+      <c r="BH15" s="35"/>
       <c r="BI15" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="60" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="10">
@@ -16492,22 +16491,22 @@
         <f t="shared" si="5"/>
         <v>1.1173522599999999</v>
       </c>
-      <c r="AX16" s="37"/>
-      <c r="AY16" s="37"/>
-      <c r="AZ16" s="33"/>
-      <c r="BA16" s="37"/>
-      <c r="BB16" s="33"/>
-      <c r="BC16" s="37"/>
-      <c r="BD16" s="33"/>
-      <c r="BE16" s="32"/>
-      <c r="BF16" s="33"/>
-      <c r="BG16" s="37"/>
-      <c r="BH16" s="33"/>
+      <c r="AX16" s="36"/>
+      <c r="AY16" s="36"/>
+      <c r="AZ16" s="37"/>
+      <c r="BA16" s="36"/>
+      <c r="BB16" s="37"/>
+      <c r="BC16" s="36"/>
+      <c r="BD16" s="37"/>
+      <c r="BE16" s="67"/>
+      <c r="BF16" s="37"/>
+      <c r="BG16" s="36"/>
+      <c r="BH16" s="37"/>
       <c r="BI16" s="48"/>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A17" s="54"/>
-      <c r="B17" s="51"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="5">
         <v>100000</v>
       </c>
@@ -16650,22 +16649,22 @@
         <f t="shared" si="5"/>
         <v>4.3320717799999997</v>
       </c>
-      <c r="AX17" s="37"/>
-      <c r="AY17" s="37"/>
-      <c r="AZ17" s="33"/>
-      <c r="BA17" s="37"/>
-      <c r="BB17" s="33"/>
-      <c r="BC17" s="37"/>
-      <c r="BD17" s="33"/>
-      <c r="BE17" s="32"/>
-      <c r="BF17" s="33"/>
-      <c r="BG17" s="37"/>
-      <c r="BH17" s="33"/>
+      <c r="AX17" s="36"/>
+      <c r="AY17" s="36"/>
+      <c r="AZ17" s="37"/>
+      <c r="BA17" s="36"/>
+      <c r="BB17" s="37"/>
+      <c r="BC17" s="36"/>
+      <c r="BD17" s="37"/>
+      <c r="BE17" s="67"/>
+      <c r="BF17" s="37"/>
+      <c r="BG17" s="36"/>
+      <c r="BH17" s="37"/>
       <c r="BI17" s="48"/>
     </row>
     <row r="18" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
-      <c r="B18" s="51"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="5">
         <v>175000</v>
       </c>
@@ -16808,22 +16807,22 @@
         <f t="shared" si="5"/>
         <v>13.35462506</v>
       </c>
-      <c r="AX18" s="37"/>
-      <c r="AY18" s="37"/>
-      <c r="AZ18" s="33"/>
-      <c r="BA18" s="37"/>
-      <c r="BB18" s="33"/>
-      <c r="BC18" s="37"/>
-      <c r="BD18" s="33"/>
-      <c r="BE18" s="32"/>
-      <c r="BF18" s="33"/>
-      <c r="BG18" s="37"/>
-      <c r="BH18" s="33"/>
+      <c r="AX18" s="36"/>
+      <c r="AY18" s="36"/>
+      <c r="AZ18" s="37"/>
+      <c r="BA18" s="36"/>
+      <c r="BB18" s="37"/>
+      <c r="BC18" s="36"/>
+      <c r="BD18" s="37"/>
+      <c r="BE18" s="67"/>
+      <c r="BF18" s="37"/>
+      <c r="BG18" s="36"/>
+      <c r="BH18" s="37"/>
       <c r="BI18" s="48"/>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="5">
         <v>300000</v>
       </c>
@@ -16966,22 +16965,22 @@
         <f t="shared" si="5"/>
         <v>41.141370479999999</v>
       </c>
-      <c r="AX19" s="37"/>
-      <c r="AY19" s="37"/>
-      <c r="AZ19" s="33"/>
-      <c r="BA19" s="37"/>
-      <c r="BB19" s="33"/>
-      <c r="BC19" s="37"/>
-      <c r="BD19" s="33"/>
-      <c r="BE19" s="32"/>
-      <c r="BF19" s="33"/>
-      <c r="BG19" s="37"/>
-      <c r="BH19" s="33"/>
+      <c r="AX19" s="36"/>
+      <c r="AY19" s="36"/>
+      <c r="AZ19" s="37"/>
+      <c r="BA19" s="36"/>
+      <c r="BB19" s="37"/>
+      <c r="BC19" s="36"/>
+      <c r="BD19" s="37"/>
+      <c r="BE19" s="67"/>
+      <c r="BF19" s="37"/>
+      <c r="BG19" s="36"/>
+      <c r="BH19" s="37"/>
       <c r="BI19" s="48"/>
     </row>
     <row r="20" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="54"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="5">
         <v>425000</v>
       </c>
@@ -17126,20 +17125,20 @@
       </c>
       <c r="AX20" s="38"/>
       <c r="AY20" s="38"/>
-      <c r="AZ20" s="35"/>
+      <c r="AZ20" s="39"/>
       <c r="BA20" s="38"/>
-      <c r="BB20" s="35"/>
+      <c r="BB20" s="39"/>
       <c r="BC20" s="38"/>
-      <c r="BD20" s="35"/>
-      <c r="BE20" s="34"/>
-      <c r="BF20" s="35"/>
+      <c r="BD20" s="39"/>
+      <c r="BE20" s="68"/>
+      <c r="BF20" s="39"/>
       <c r="BG20" s="38"/>
-      <c r="BH20" s="35"/>
+      <c r="BH20" s="39"/>
       <c r="BI20" s="49"/>
     </row>
     <row r="21" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="55"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="6">
         <v>550000</v>
       </c>
@@ -17282,38 +17281,38 @@
         <f t="shared" si="5"/>
         <v>135.94702348000001</v>
       </c>
-      <c r="AX21" s="46" t="s">
+      <c r="AX21" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="AY21" s="36" t="s">
+      <c r="AY21" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="AZ21" s="31"/>
-      <c r="BA21" s="36" t="s">
+      <c r="AZ21" s="35"/>
+      <c r="BA21" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="BB21" s="31"/>
-      <c r="BC21" s="36" t="s">
+      <c r="BB21" s="35"/>
+      <c r="BC21" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="BD21" s="31"/>
-      <c r="BE21" s="30" t="s">
+      <c r="BD21" s="35"/>
+      <c r="BE21" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="BF21" s="31"/>
-      <c r="BG21" s="46" t="s">
+      <c r="BF21" s="35"/>
+      <c r="BG21" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="BH21" s="31"/>
+      <c r="BH21" s="35"/>
       <c r="BI21" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="10">
@@ -17454,22 +17453,22 @@
         <f t="shared" si="5"/>
         <v>2.1009380000000001E-2</v>
       </c>
-      <c r="AX22" s="37"/>
-      <c r="AY22" s="37"/>
-      <c r="AZ22" s="33"/>
-      <c r="BA22" s="37"/>
-      <c r="BB22" s="33"/>
-      <c r="BC22" s="37"/>
-      <c r="BD22" s="33"/>
-      <c r="BE22" s="32"/>
-      <c r="BF22" s="33"/>
-      <c r="BG22" s="37"/>
-      <c r="BH22" s="33"/>
+      <c r="AX22" s="36"/>
+      <c r="AY22" s="36"/>
+      <c r="AZ22" s="37"/>
+      <c r="BA22" s="36"/>
+      <c r="BB22" s="37"/>
+      <c r="BC22" s="36"/>
+      <c r="BD22" s="37"/>
+      <c r="BE22" s="67"/>
+      <c r="BF22" s="37"/>
+      <c r="BG22" s="36"/>
+      <c r="BH22" s="37"/>
       <c r="BI22" s="48"/>
     </row>
     <row r="23" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A23" s="54"/>
-      <c r="B23" s="51"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="5">
         <v>100000</v>
       </c>
@@ -17612,22 +17611,22 @@
         <f t="shared" si="5"/>
         <v>3.9191080000000003E-2</v>
       </c>
-      <c r="AX23" s="37"/>
-      <c r="AY23" s="37"/>
-      <c r="AZ23" s="33"/>
-      <c r="BA23" s="37"/>
-      <c r="BB23" s="33"/>
-      <c r="BC23" s="37"/>
-      <c r="BD23" s="33"/>
-      <c r="BE23" s="32"/>
-      <c r="BF23" s="33"/>
-      <c r="BG23" s="37"/>
-      <c r="BH23" s="33"/>
+      <c r="AX23" s="36"/>
+      <c r="AY23" s="36"/>
+      <c r="AZ23" s="37"/>
+      <c r="BA23" s="36"/>
+      <c r="BB23" s="37"/>
+      <c r="BC23" s="36"/>
+      <c r="BD23" s="37"/>
+      <c r="BE23" s="67"/>
+      <c r="BF23" s="37"/>
+      <c r="BG23" s="36"/>
+      <c r="BH23" s="37"/>
       <c r="BI23" s="48"/>
     </row>
     <row r="24" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A24" s="54"/>
-      <c r="B24" s="51"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="5">
         <v>175000</v>
       </c>
@@ -17770,22 +17769,22 @@
         <f t="shared" si="5"/>
         <v>6.838284E-2</v>
       </c>
-      <c r="AX24" s="37"/>
-      <c r="AY24" s="37"/>
-      <c r="AZ24" s="33"/>
-      <c r="BA24" s="37"/>
-      <c r="BB24" s="33"/>
-      <c r="BC24" s="37"/>
-      <c r="BD24" s="33"/>
-      <c r="BE24" s="32"/>
-      <c r="BF24" s="33"/>
-      <c r="BG24" s="37"/>
-      <c r="BH24" s="33"/>
+      <c r="AX24" s="36"/>
+      <c r="AY24" s="36"/>
+      <c r="AZ24" s="37"/>
+      <c r="BA24" s="36"/>
+      <c r="BB24" s="37"/>
+      <c r="BC24" s="36"/>
+      <c r="BD24" s="37"/>
+      <c r="BE24" s="67"/>
+      <c r="BF24" s="37"/>
+      <c r="BG24" s="36"/>
+      <c r="BH24" s="37"/>
       <c r="BI24" s="48"/>
     </row>
     <row r="25" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
-      <c r="B25" s="51"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="5">
         <v>300000</v>
       </c>
@@ -17928,22 +17927,22 @@
         <f t="shared" si="5"/>
         <v>0.11834768</v>
       </c>
-      <c r="AX25" s="37"/>
-      <c r="AY25" s="37"/>
-      <c r="AZ25" s="33"/>
-      <c r="BA25" s="37"/>
-      <c r="BB25" s="33"/>
-      <c r="BC25" s="37"/>
-      <c r="BD25" s="33"/>
-      <c r="BE25" s="32"/>
-      <c r="BF25" s="33"/>
-      <c r="BG25" s="37"/>
-      <c r="BH25" s="33"/>
+      <c r="AX25" s="36"/>
+      <c r="AY25" s="36"/>
+      <c r="AZ25" s="37"/>
+      <c r="BA25" s="36"/>
+      <c r="BB25" s="37"/>
+      <c r="BC25" s="36"/>
+      <c r="BD25" s="37"/>
+      <c r="BE25" s="67"/>
+      <c r="BF25" s="37"/>
+      <c r="BG25" s="36"/>
+      <c r="BH25" s="37"/>
       <c r="BI25" s="48"/>
     </row>
     <row r="26" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="54"/>
-      <c r="B26" s="51"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="5">
         <v>425000</v>
       </c>
@@ -18088,20 +18087,20 @@
       </c>
       <c r="AX26" s="38"/>
       <c r="AY26" s="38"/>
-      <c r="AZ26" s="35"/>
+      <c r="AZ26" s="39"/>
       <c r="BA26" s="38"/>
-      <c r="BB26" s="35"/>
+      <c r="BB26" s="39"/>
       <c r="BC26" s="38"/>
-      <c r="BD26" s="35"/>
-      <c r="BE26" s="34"/>
-      <c r="BF26" s="35"/>
+      <c r="BD26" s="39"/>
+      <c r="BE26" s="68"/>
+      <c r="BF26" s="39"/>
       <c r="BG26" s="38"/>
-      <c r="BH26" s="35"/>
+      <c r="BH26" s="39"/>
       <c r="BI26" s="49"/>
     </row>
     <row r="27" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="55"/>
-      <c r="B27" s="52"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="6">
         <v>550000</v>
       </c>
@@ -18244,38 +18243,38 @@
         <f t="shared" si="5"/>
         <v>0.21743744000000001</v>
       </c>
-      <c r="AX27" s="46" t="s">
+      <c r="AX27" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AY27" s="36" t="s">
+      <c r="AY27" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="AZ27" s="31"/>
-      <c r="BA27" s="36" t="s">
+      <c r="AZ27" s="35"/>
+      <c r="BA27" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BB27" s="31"/>
-      <c r="BC27" s="36" t="s">
+      <c r="BB27" s="35"/>
+      <c r="BC27" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="BD27" s="31"/>
-      <c r="BE27" s="30" t="s">
+      <c r="BD27" s="35"/>
+      <c r="BE27" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="BF27" s="31"/>
-      <c r="BG27" s="58" t="s">
+      <c r="BF27" s="35"/>
+      <c r="BG27" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="BH27" s="59"/>
+      <c r="BH27" s="42"/>
       <c r="BI27" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="60" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="10">
@@ -18416,22 +18415,22 @@
         <f t="shared" si="5"/>
         <v>2.1247800000000002E-3</v>
       </c>
-      <c r="AX28" s="37"/>
-      <c r="AY28" s="37"/>
-      <c r="AZ28" s="33"/>
-      <c r="BA28" s="37"/>
-      <c r="BB28" s="33"/>
-      <c r="BC28" s="37"/>
-      <c r="BD28" s="33"/>
-      <c r="BE28" s="32"/>
-      <c r="BF28" s="33"/>
-      <c r="BG28" s="60"/>
-      <c r="BH28" s="61"/>
+      <c r="AX28" s="36"/>
+      <c r="AY28" s="36"/>
+      <c r="AZ28" s="37"/>
+      <c r="BA28" s="36"/>
+      <c r="BB28" s="37"/>
+      <c r="BC28" s="36"/>
+      <c r="BD28" s="37"/>
+      <c r="BE28" s="67"/>
+      <c r="BF28" s="37"/>
+      <c r="BG28" s="43"/>
+      <c r="BH28" s="44"/>
       <c r="BI28" s="48"/>
     </row>
     <row r="29" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A29" s="54"/>
-      <c r="B29" s="51"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="5">
         <v>100000</v>
       </c>
@@ -18574,22 +18573,22 @@
         <f t="shared" si="5"/>
         <v>4.1765199999999995E-3</v>
       </c>
-      <c r="AX29" s="37"/>
-      <c r="AY29" s="37"/>
-      <c r="AZ29" s="33"/>
-      <c r="BA29" s="37"/>
-      <c r="BB29" s="33"/>
-      <c r="BC29" s="37"/>
-      <c r="BD29" s="33"/>
-      <c r="BE29" s="32"/>
-      <c r="BF29" s="33"/>
-      <c r="BG29" s="60"/>
-      <c r="BH29" s="61"/>
+      <c r="AX29" s="36"/>
+      <c r="AY29" s="36"/>
+      <c r="AZ29" s="37"/>
+      <c r="BA29" s="36"/>
+      <c r="BB29" s="37"/>
+      <c r="BC29" s="36"/>
+      <c r="BD29" s="37"/>
+      <c r="BE29" s="67"/>
+      <c r="BF29" s="37"/>
+      <c r="BG29" s="43"/>
+      <c r="BH29" s="44"/>
       <c r="BI29" s="48"/>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A30" s="54"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="5">
         <v>175000</v>
       </c>
@@ -18732,22 +18731,22 @@
         <f t="shared" si="5"/>
         <v>7.9310400000000003E-3</v>
       </c>
-      <c r="AX30" s="37"/>
-      <c r="AY30" s="37"/>
-      <c r="AZ30" s="33"/>
-      <c r="BA30" s="37"/>
-      <c r="BB30" s="33"/>
-      <c r="BC30" s="37"/>
-      <c r="BD30" s="33"/>
-      <c r="BE30" s="32"/>
-      <c r="BF30" s="33"/>
-      <c r="BG30" s="60"/>
-      <c r="BH30" s="61"/>
+      <c r="AX30" s="36"/>
+      <c r="AY30" s="36"/>
+      <c r="AZ30" s="37"/>
+      <c r="BA30" s="36"/>
+      <c r="BB30" s="37"/>
+      <c r="BC30" s="36"/>
+      <c r="BD30" s="37"/>
+      <c r="BE30" s="67"/>
+      <c r="BF30" s="37"/>
+      <c r="BG30" s="43"/>
+      <c r="BH30" s="44"/>
       <c r="BI30" s="48"/>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A31" s="54"/>
-      <c r="B31" s="51"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="5">
         <v>300000</v>
       </c>
@@ -18890,22 +18889,22 @@
         <f t="shared" si="5"/>
         <v>1.3708639999999999E-2</v>
       </c>
-      <c r="AX31" s="37"/>
-      <c r="AY31" s="37"/>
-      <c r="AZ31" s="33"/>
-      <c r="BA31" s="37"/>
-      <c r="BB31" s="33"/>
-      <c r="BC31" s="37"/>
-      <c r="BD31" s="33"/>
-      <c r="BE31" s="32"/>
-      <c r="BF31" s="33"/>
-      <c r="BG31" s="60"/>
-      <c r="BH31" s="61"/>
+      <c r="AX31" s="36"/>
+      <c r="AY31" s="36"/>
+      <c r="AZ31" s="37"/>
+      <c r="BA31" s="36"/>
+      <c r="BB31" s="37"/>
+      <c r="BC31" s="36"/>
+      <c r="BD31" s="37"/>
+      <c r="BE31" s="67"/>
+      <c r="BF31" s="37"/>
+      <c r="BG31" s="43"/>
+      <c r="BH31" s="44"/>
       <c r="BI31" s="48"/>
     </row>
     <row r="32" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="54"/>
-      <c r="B32" s="51"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="5">
         <v>425000</v>
       </c>
@@ -19050,20 +19049,20 @@
       </c>
       <c r="AX32" s="38"/>
       <c r="AY32" s="38"/>
-      <c r="AZ32" s="35"/>
+      <c r="AZ32" s="39"/>
       <c r="BA32" s="38"/>
-      <c r="BB32" s="35"/>
+      <c r="BB32" s="39"/>
       <c r="BC32" s="38"/>
-      <c r="BD32" s="35"/>
-      <c r="BE32" s="34"/>
-      <c r="BF32" s="35"/>
-      <c r="BG32" s="62"/>
-      <c r="BH32" s="63"/>
+      <c r="BD32" s="39"/>
+      <c r="BE32" s="68"/>
+      <c r="BF32" s="39"/>
+      <c r="BG32" s="45"/>
+      <c r="BH32" s="46"/>
       <c r="BI32" s="49"/>
     </row>
     <row r="33" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="55"/>
-      <c r="B33" s="52"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="6">
         <v>550000</v>
       </c>
@@ -19206,38 +19205,38 @@
         <f t="shared" si="5"/>
         <v>2.6853200000000001E-2</v>
       </c>
-      <c r="AX33" s="46" t="s">
+      <c r="AX33" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AY33" s="36" t="s">
+      <c r="AY33" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="AZ33" s="31"/>
-      <c r="BA33" s="36" t="s">
+      <c r="AZ33" s="35"/>
+      <c r="BA33" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BB33" s="31"/>
-      <c r="BC33" s="36" t="s">
+      <c r="BB33" s="35"/>
+      <c r="BC33" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="BD33" s="31"/>
-      <c r="BE33" s="30" t="s">
+      <c r="BD33" s="35"/>
+      <c r="BE33" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BF33" s="31"/>
-      <c r="BG33" s="58" t="s">
+      <c r="BF33" s="35"/>
+      <c r="BG33" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="BH33" s="59"/>
+      <c r="BH33" s="42"/>
       <c r="BI33" s="48" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="7">
@@ -19378,22 +19377,22 @@
         <f t="shared" si="5"/>
         <v>1.7947400000000002E-3</v>
       </c>
-      <c r="AX34" s="37"/>
-      <c r="AY34" s="37"/>
-      <c r="AZ34" s="33"/>
-      <c r="BA34" s="37"/>
-      <c r="BB34" s="33"/>
-      <c r="BC34" s="37"/>
-      <c r="BD34" s="33"/>
-      <c r="BE34" s="32"/>
-      <c r="BF34" s="33"/>
-      <c r="BG34" s="60"/>
-      <c r="BH34" s="61"/>
+      <c r="AX34" s="36"/>
+      <c r="AY34" s="36"/>
+      <c r="AZ34" s="37"/>
+      <c r="BA34" s="36"/>
+      <c r="BB34" s="37"/>
+      <c r="BC34" s="36"/>
+      <c r="BD34" s="37"/>
+      <c r="BE34" s="67"/>
+      <c r="BF34" s="37"/>
+      <c r="BG34" s="43"/>
+      <c r="BH34" s="44"/>
       <c r="BI34" s="48"/>
     </row>
     <row r="35" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A35" s="54"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="5">
         <v>100000</v>
       </c>
@@ -19536,22 +19535,22 @@
         <f t="shared" si="5"/>
         <v>3.2638199999999997E-3</v>
       </c>
-      <c r="AX35" s="37"/>
-      <c r="AY35" s="37"/>
-      <c r="AZ35" s="33"/>
-      <c r="BA35" s="37"/>
-      <c r="BB35" s="33"/>
-      <c r="BC35" s="37"/>
-      <c r="BD35" s="33"/>
-      <c r="BE35" s="32"/>
-      <c r="BF35" s="33"/>
-      <c r="BG35" s="60"/>
-      <c r="BH35" s="61"/>
+      <c r="AX35" s="36"/>
+      <c r="AY35" s="36"/>
+      <c r="AZ35" s="37"/>
+      <c r="BA35" s="36"/>
+      <c r="BB35" s="37"/>
+      <c r="BC35" s="36"/>
+      <c r="BD35" s="37"/>
+      <c r="BE35" s="67"/>
+      <c r="BF35" s="37"/>
+      <c r="BG35" s="43"/>
+      <c r="BH35" s="44"/>
       <c r="BI35" s="48"/>
     </row>
     <row r="36" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A36" s="54"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="5">
         <v>175000</v>
       </c>
@@ -19694,22 +19693,22 @@
         <f t="shared" si="5"/>
         <v>6.2572799999999996E-3</v>
       </c>
-      <c r="AX36" s="37"/>
-      <c r="AY36" s="37"/>
-      <c r="AZ36" s="33"/>
-      <c r="BA36" s="37"/>
-      <c r="BB36" s="33"/>
-      <c r="BC36" s="37"/>
-      <c r="BD36" s="33"/>
-      <c r="BE36" s="32"/>
-      <c r="BF36" s="33"/>
-      <c r="BG36" s="60"/>
-      <c r="BH36" s="61"/>
+      <c r="AX36" s="36"/>
+      <c r="AY36" s="36"/>
+      <c r="AZ36" s="37"/>
+      <c r="BA36" s="36"/>
+      <c r="BB36" s="37"/>
+      <c r="BC36" s="36"/>
+      <c r="BD36" s="37"/>
+      <c r="BE36" s="67"/>
+      <c r="BF36" s="37"/>
+      <c r="BG36" s="43"/>
+      <c r="BH36" s="44"/>
       <c r="BI36" s="48"/>
     </row>
     <row r="37" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A37" s="54"/>
-      <c r="B37" s="51"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="5">
         <v>300000</v>
       </c>
@@ -19852,22 +19851,22 @@
         <f t="shared" si="5"/>
         <v>1.0778959999999999E-2</v>
       </c>
-      <c r="AX37" s="37"/>
-      <c r="AY37" s="37"/>
-      <c r="AZ37" s="33"/>
-      <c r="BA37" s="37"/>
-      <c r="BB37" s="33"/>
-      <c r="BC37" s="37"/>
-      <c r="BD37" s="33"/>
-      <c r="BE37" s="32"/>
-      <c r="BF37" s="33"/>
-      <c r="BG37" s="60"/>
-      <c r="BH37" s="61"/>
+      <c r="AX37" s="36"/>
+      <c r="AY37" s="36"/>
+      <c r="AZ37" s="37"/>
+      <c r="BA37" s="36"/>
+      <c r="BB37" s="37"/>
+      <c r="BC37" s="36"/>
+      <c r="BD37" s="37"/>
+      <c r="BE37" s="67"/>
+      <c r="BF37" s="37"/>
+      <c r="BG37" s="43"/>
+      <c r="BH37" s="44"/>
       <c r="BI37" s="48"/>
     </row>
     <row r="38" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="54"/>
-      <c r="B38" s="51"/>
+      <c r="A38" s="57"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="5">
         <v>425000</v>
       </c>
@@ -20012,20 +20011,20 @@
       </c>
       <c r="AX38" s="38"/>
       <c r="AY38" s="38"/>
-      <c r="AZ38" s="35"/>
+      <c r="AZ38" s="39"/>
       <c r="BA38" s="38"/>
-      <c r="BB38" s="35"/>
+      <c r="BB38" s="39"/>
       <c r="BC38" s="38"/>
-      <c r="BD38" s="35"/>
-      <c r="BE38" s="34"/>
-      <c r="BF38" s="35"/>
-      <c r="BG38" s="62"/>
-      <c r="BH38" s="63"/>
+      <c r="BD38" s="39"/>
+      <c r="BE38" s="68"/>
+      <c r="BF38" s="39"/>
+      <c r="BG38" s="45"/>
+      <c r="BH38" s="46"/>
       <c r="BI38" s="49"/>
     </row>
     <row r="39" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="55"/>
-      <c r="B39" s="52"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="6">
         <v>550000</v>
       </c>
@@ -20210,7 +20209,7 @@
         <f>AI10/AI4</f>
         <v>0.2259003724994392</v>
       </c>
-      <c r="AS46" s="65">
+      <c r="AS46" s="30">
         <f>AI4/AI10</f>
         <v>4.4267301949777993</v>
       </c>
@@ -20221,22 +20220,22 @@
         <v>9.9029751783332961E-4</v>
       </c>
       <c r="AK47">
-        <f t="shared" ref="AK47:AK51" si="34">AI29/AI5</f>
+        <f t="shared" ref="AK47:AK50" si="34">AI29/AI5</f>
         <v>4.8393022560199697E-4</v>
       </c>
       <c r="AM47">
-        <f t="shared" ref="AM47:AM51" si="35">AI23/AI5</f>
+        <f t="shared" ref="AM47:AM50" si="35">AI23/AI5</f>
         <v>3.0252982317538566E-3</v>
       </c>
       <c r="AO47">
-        <f t="shared" ref="AO47:AO51" si="36">AI17/AI5</f>
+        <f t="shared" ref="AO47:AO50" si="36">AI17/AI5</f>
         <v>0.13502435798277596</v>
       </c>
       <c r="AQ47">
         <f t="shared" ref="AQ47:AQ51" si="37">AI11/AI5</f>
         <v>0.21136013787000474</v>
       </c>
-      <c r="AS47" s="65">
+      <c r="AS47" s="30">
         <f t="shared" ref="AS47:AS51" si="38">AI5/AI11</f>
         <v>4.7312611075937205</v>
       </c>
@@ -20262,7 +20261,7 @@
         <f t="shared" si="37"/>
         <v>0.22063037682291717</v>
       </c>
-      <c r="AS48" s="65">
+      <c r="AS48" s="30">
         <f t="shared" si="38"/>
         <v>4.5324674435135561</v>
       </c>
@@ -20288,7 +20287,7 @@
         <f t="shared" si="37"/>
         <v>0.20901427367520201</v>
       </c>
-      <c r="AS49" s="65">
+      <c r="AS49" s="30">
         <f t="shared" si="38"/>
         <v>4.7843622467332123</v>
       </c>
@@ -20314,7 +20313,7 @@
         <f t="shared" si="37"/>
         <v>0.21679792479799201</v>
       </c>
-      <c r="AS50" s="65">
+      <c r="AS50" s="30">
         <f t="shared" si="38"/>
         <v>4.6125902770138607</v>
       </c>
@@ -20340,7 +20339,7 @@
         <f t="shared" si="37"/>
         <v>0.2218091667444945</v>
       </c>
-      <c r="AS51" s="65">
+      <c r="AS51" s="30">
         <f t="shared" si="38"/>
         <v>4.5083799496524684</v>
       </c>
@@ -20413,7 +20412,7 @@
         <v>1.5653482158898053</v>
       </c>
       <c r="AS54">
-        <f t="shared" ref="AS54:AS58" si="43">AI5/AI17</f>
+        <f t="shared" ref="AS54:AS57" si="43">AI5/AI17</f>
         <v>7.406071133680654</v>
       </c>
     </row>
@@ -20442,12 +20441,12 @@
         <f t="shared" si="43"/>
         <v>7.1980224023610671</v>
       </c>
-      <c r="AV55" s="64" t="s">
+      <c r="AV55" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="AW55" s="64"/>
-      <c r="AX55" s="64"/>
-      <c r="AY55" s="64"/>
+      <c r="AW55" s="40"/>
+      <c r="AX55" s="40"/>
+      <c r="AY55" s="40"/>
     </row>
     <row r="56" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI56">
@@ -20474,10 +20473,10 @@
         <f t="shared" si="43"/>
         <v>7.4891872009526663</v>
       </c>
-      <c r="AV56" s="64"/>
-      <c r="AW56" s="64"/>
-      <c r="AX56" s="64"/>
-      <c r="AY56" s="64"/>
+      <c r="AV56" s="40"/>
+      <c r="AW56" s="40"/>
+      <c r="AX56" s="40"/>
+      <c r="AY56" s="40"/>
     </row>
     <row r="57" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI57">
@@ -20504,10 +20503,10 @@
         <f t="shared" si="43"/>
         <v>7.6305177539244724</v>
       </c>
-      <c r="AV57" s="64"/>
-      <c r="AW57" s="64"/>
-      <c r="AX57" s="64"/>
-      <c r="AY57" s="64"/>
+      <c r="AV57" s="40"/>
+      <c r="AW57" s="40"/>
+      <c r="AX57" s="40"/>
+      <c r="AY57" s="40"/>
     </row>
     <row r="58" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI58">
@@ -20534,10 +20533,10 @@
         <f>AI9/AI21</f>
         <v>7.4634895127569365</v>
       </c>
-      <c r="AV58" s="64"/>
-      <c r="AW58" s="64"/>
-      <c r="AX58" s="64"/>
-      <c r="AY58" s="64"/>
+      <c r="AV58" s="40"/>
+      <c r="AW58" s="40"/>
+      <c r="AX58" s="40"/>
+      <c r="AY58" s="40"/>
     </row>
     <row r="59" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI59" t="s">
@@ -20558,10 +20557,10 @@
       <c r="AS59" t="s">
         <v>64</v>
       </c>
-      <c r="AV59" s="64"/>
-      <c r="AW59" s="64"/>
-      <c r="AX59" s="64"/>
-      <c r="AY59" s="64"/>
+      <c r="AV59" s="40"/>
+      <c r="AW59" s="40"/>
+      <c r="AX59" s="40"/>
+      <c r="AY59" s="40"/>
     </row>
     <row r="60" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI60">
@@ -20576,7 +20575,7 @@
         <f>AI22/AI16</f>
         <v>4.8681674543527363E-2</v>
       </c>
-      <c r="AO60" s="68">
+      <c r="AO60" s="33">
         <f>AI16/AI22</f>
         <v>20.541610562427916</v>
       </c>
@@ -20584,14 +20583,14 @@
         <f>AI10/AI22</f>
         <v>31.859764040207715</v>
       </c>
-      <c r="AS60" s="69">
+      <c r="AS60">
         <f>AI4/AI22</f>
         <v>141.03457948165538</v>
       </c>
-      <c r="AV60" s="64"/>
-      <c r="AW60" s="64"/>
-      <c r="AX60" s="64"/>
-      <c r="AY60" s="64"/>
+      <c r="AV60" s="40"/>
+      <c r="AW60" s="40"/>
+      <c r="AX60" s="40"/>
+      <c r="AY60" s="40"/>
     </row>
     <row r="61" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI61">
@@ -20610,7 +20609,7 @@
         <f t="shared" ref="AO61:AO65" si="46">AI17/AI23</f>
         <v>44.631751199120046</v>
       </c>
-      <c r="AQ61" s="69">
+      <c r="AQ61">
         <f t="shared" ref="AQ61:AQ65" si="47">AI11/AI23</f>
         <v>69.86423211158025</v>
       </c>
@@ -20618,10 +20617,10 @@
         <f t="shared" ref="AS61:AS65" si="48">AI5/AI23</f>
         <v>330.54592420141995</v>
       </c>
-      <c r="AV61" s="64"/>
-      <c r="AW61" s="64"/>
-      <c r="AX61" s="64"/>
-      <c r="AY61" s="64"/>
+      <c r="AV61" s="40"/>
+      <c r="AW61" s="40"/>
+      <c r="AX61" s="40"/>
+      <c r="AY61" s="40"/>
     </row>
     <row r="62" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI62">
@@ -20636,11 +20635,11 @@
         <f t="shared" si="45"/>
         <v>1.2254110248346925E-2</v>
       </c>
-      <c r="AO62" s="67">
+      <c r="AO62" s="32">
         <f t="shared" si="46"/>
         <v>81.605272005358344</v>
       </c>
-      <c r="AQ62" s="69">
+      <c r="AQ62">
         <f t="shared" si="47"/>
         <v>129.59752791737418</v>
       </c>
@@ -20648,10 +20647,10 @@
         <f t="shared" si="48"/>
         <v>587.39657604533772</v>
       </c>
-      <c r="AV62" s="64"/>
-      <c r="AW62" s="64"/>
-      <c r="AX62" s="64"/>
-      <c r="AY62" s="64"/>
+      <c r="AV62" s="40"/>
+      <c r="AW62" s="40"/>
+      <c r="AX62" s="40"/>
+      <c r="AY62" s="40"/>
     </row>
     <row r="63" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI63">
@@ -20666,7 +20665,7 @@
         <f t="shared" si="45"/>
         <v>7.266679938985463E-3</v>
       </c>
-      <c r="AO63" s="69">
+      <c r="AO63">
         <f t="shared" si="46"/>
         <v>137.61442755102476</v>
       </c>
@@ -20678,10 +20677,10 @@
         <f t="shared" si="48"/>
         <v>1030.6202094815626</v>
       </c>
-      <c r="AV63" s="64"/>
-      <c r="AW63" s="64"/>
-      <c r="AX63" s="64"/>
-      <c r="AY63" s="64"/>
+      <c r="AV63" s="40"/>
+      <c r="AW63" s="40"/>
+      <c r="AX63" s="40"/>
+      <c r="AY63" s="40"/>
     </row>
     <row r="64" spans="35:51" x14ac:dyDescent="0.35">
       <c r="AI64">
@@ -20764,7 +20763,7 @@
         <f>AI28/AI22</f>
         <v>0.13658284205534707</v>
       </c>
-      <c r="AM67" s="65">
+      <c r="AM67" s="30">
         <f>AI22/AI28</f>
         <v>7.3215638578876021</v>
       </c>
@@ -20790,7 +20789,7 @@
         <f t="shared" ref="AK68:AK72" si="49">AI29/AI23</f>
         <v>0.15996116367061375</v>
       </c>
-      <c r="AM68" s="65">
+      <c r="AM68" s="30">
         <f t="shared" ref="AM68:AM72" si="50">AI23/AI29</f>
         <v>6.2515174124337074</v>
       </c>
@@ -20816,7 +20815,7 @@
         <f t="shared" si="49"/>
         <v>0.16649278326461553</v>
       </c>
-      <c r="AM69" s="65">
+      <c r="AM69" s="30">
         <f t="shared" si="50"/>
         <v>6.0062663401491019</v>
       </c>
@@ -20842,7 +20841,7 @@
         <f t="shared" si="49"/>
         <v>0.17138671361228405</v>
       </c>
-      <c r="AM70" s="65">
+      <c r="AM70" s="30">
         <f t="shared" si="50"/>
         <v>5.8347580096682909</v>
       </c>
@@ -20868,7 +20867,7 @@
         <f t="shared" si="49"/>
         <v>0.17669534752219559</v>
       </c>
-      <c r="AM71" s="65">
+      <c r="AM71" s="30">
         <f t="shared" si="50"/>
         <v>5.6594585767142789</v>
       </c>
@@ -20894,7 +20893,7 @@
         <f t="shared" si="49"/>
         <v>0.17989151895950645</v>
       </c>
-      <c r="AM72" s="65">
+      <c r="AM72" s="30">
         <f t="shared" si="50"/>
         <v>5.5589057548905334</v>
       </c>
@@ -20932,7 +20931,7 @@
       </c>
     </row>
     <row r="74" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI74" s="65">
+      <c r="AI74" s="30">
         <f>$AI$34/AI28</f>
         <v>2.0397447506174951</v>
       </c>
@@ -20944,11 +20943,11 @@
         <f>AI22/AI34</f>
         <v>3.5894510112949836</v>
       </c>
-      <c r="AO74" s="69">
+      <c r="AO74">
         <f>AI16/AI34</f>
         <v>73.733104806934605</v>
       </c>
-      <c r="AQ74" s="67">
+      <c r="AQ74" s="32">
         <f>AI10/AI34</f>
         <v>114.35906225374313</v>
       </c>
@@ -20958,7 +20957,7 @@
       </c>
     </row>
     <row r="75" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI75" s="65">
+      <c r="AI75" s="30">
         <f>$AI$35/AI29</f>
         <v>2.0463642596438865</v>
       </c>
@@ -20970,7 +20969,7 @@
         <f t="shared" ref="AM75:AM79" si="55">AI23/AI35</f>
         <v>3.0549387202069354</v>
       </c>
-      <c r="AO75" s="69">
+      <c r="AO75">
         <f t="shared" ref="AO75:AO79" si="56">AI17/AI35</f>
         <v>136.34726488883416</v>
       </c>
@@ -20984,7 +20983,7 @@
       </c>
     </row>
     <row r="76" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI76" s="65">
+      <c r="AI76" s="30">
         <f>$AI$36/AI30</f>
         <v>2.1020281764108186</v>
       </c>
@@ -21010,7 +21009,7 @@
       </c>
     </row>
     <row r="77" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI77" s="65">
+      <c r="AI77" s="30">
         <f>$AI$37/AI31</f>
         <v>2.2399834795483669</v>
       </c>
@@ -21036,7 +21035,7 @@
       </c>
     </row>
     <row r="78" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI78" s="65">
+      <c r="AI78" s="30">
         <f>$AI$38/AI32</f>
         <v>2.2206113212485517</v>
       </c>
@@ -21062,7 +21061,7 @@
       </c>
     </row>
     <row r="79" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI79" s="65">
+      <c r="AI79" s="30">
         <f>$AI$39/AI33</f>
         <v>2.2788448148022686</v>
       </c>
@@ -21093,58 +21092,79 @@
       </c>
     </row>
     <row r="86" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO86" s="66">
+      <c r="AO86" s="31">
         <f>AO34/LOG(C34, 2)</f>
         <v>7.0631991928678879E-5</v>
       </c>
     </row>
     <row r="87" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO87" s="66">
+      <c r="AO87" s="31">
         <f t="shared" ref="AO87:AO91" si="59">AO35/LOG(C35, 2)</f>
         <v>1.377693878155776E-4</v>
       </c>
     </row>
     <row r="88" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO88" s="66">
+      <c r="AO88" s="31">
         <f t="shared" si="59"/>
         <v>2.3395654113913096E-4</v>
       </c>
     </row>
     <row r="89" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO89" s="66">
+      <c r="AO89" s="31">
         <f t="shared" si="59"/>
         <v>3.9732991205526619E-4</v>
       </c>
     </row>
     <row r="90" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO90" s="66">
+      <c r="AO90" s="31">
         <f t="shared" si="59"/>
         <v>5.4442657924767943E-4</v>
       </c>
     </row>
     <row r="91" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO91" s="66">
+      <c r="AO91" s="31">
         <f t="shared" si="59"/>
         <v>7.266509839790635E-4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="BG3:BH8"/>
-    <mergeCell ref="BG1:BH2"/>
-    <mergeCell ref="AV55:AY63"/>
-    <mergeCell ref="BG33:BH38"/>
-    <mergeCell ref="BG27:BH32"/>
-    <mergeCell ref="BG21:BH26"/>
-    <mergeCell ref="BG15:BH20"/>
-    <mergeCell ref="BG9:BH14"/>
-    <mergeCell ref="BI27:BI32"/>
-    <mergeCell ref="BI33:BI38"/>
-    <mergeCell ref="BI1:BI2"/>
-    <mergeCell ref="BI3:BI8"/>
-    <mergeCell ref="BI9:BI14"/>
-    <mergeCell ref="BI15:BI20"/>
-    <mergeCell ref="BI21:BI26"/>
+    <mergeCell ref="BE27:BF32"/>
+    <mergeCell ref="BA33:BB38"/>
+    <mergeCell ref="BC33:BD38"/>
+    <mergeCell ref="BE33:BF38"/>
+    <mergeCell ref="BE3:BF8"/>
+    <mergeCell ref="BC9:BD14"/>
+    <mergeCell ref="BE9:BF14"/>
+    <mergeCell ref="BC15:BD20"/>
+    <mergeCell ref="BE15:BF20"/>
+    <mergeCell ref="BC21:BD26"/>
+    <mergeCell ref="BE21:BF26"/>
+    <mergeCell ref="BC27:BD32"/>
+    <mergeCell ref="BC3:BD8"/>
+    <mergeCell ref="AY33:AZ38"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="AY9:AZ14"/>
+    <mergeCell ref="AY15:AZ20"/>
+    <mergeCell ref="AY21:AZ26"/>
+    <mergeCell ref="AY27:AZ32"/>
+    <mergeCell ref="BA9:BB14"/>
+    <mergeCell ref="BA15:BB20"/>
+    <mergeCell ref="BA21:BB26"/>
+    <mergeCell ref="BA27:BB32"/>
+    <mergeCell ref="AD2:AI2"/>
+    <mergeCell ref="AJ2:AO2"/>
+    <mergeCell ref="AP2:AU2"/>
+    <mergeCell ref="AY1:BD1"/>
+    <mergeCell ref="BE1:BF2"/>
+    <mergeCell ref="AC22:AC27"/>
+    <mergeCell ref="AC28:AC33"/>
+    <mergeCell ref="AC34:AC39"/>
+    <mergeCell ref="AC4:AC9"/>
+    <mergeCell ref="AC10:AC15"/>
+    <mergeCell ref="AC16:AC21"/>
     <mergeCell ref="U2:AA2"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="N2:T2"/>
@@ -21160,50 +21180,29 @@
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="B28:B33"/>
-    <mergeCell ref="AC22:AC27"/>
-    <mergeCell ref="AC28:AC33"/>
-    <mergeCell ref="AC34:AC39"/>
-    <mergeCell ref="AC4:AC9"/>
-    <mergeCell ref="AC10:AC15"/>
-    <mergeCell ref="AC16:AC21"/>
+    <mergeCell ref="BI27:BI32"/>
+    <mergeCell ref="BI33:BI38"/>
+    <mergeCell ref="BI1:BI2"/>
+    <mergeCell ref="BI3:BI8"/>
+    <mergeCell ref="BI9:BI14"/>
+    <mergeCell ref="BI15:BI20"/>
+    <mergeCell ref="BI21:BI26"/>
+    <mergeCell ref="BG3:BH8"/>
+    <mergeCell ref="BG1:BH2"/>
+    <mergeCell ref="AV55:AY63"/>
+    <mergeCell ref="BG33:BH38"/>
+    <mergeCell ref="BG27:BH32"/>
+    <mergeCell ref="BG21:BH26"/>
+    <mergeCell ref="BG15:BH20"/>
+    <mergeCell ref="BG9:BH14"/>
     <mergeCell ref="AX21:AX26"/>
     <mergeCell ref="AX27:AX32"/>
     <mergeCell ref="AX33:AX38"/>
-    <mergeCell ref="AD2:AI2"/>
-    <mergeCell ref="AJ2:AO2"/>
-    <mergeCell ref="AP2:AU2"/>
-    <mergeCell ref="AY1:BD1"/>
-    <mergeCell ref="BE1:BF2"/>
     <mergeCell ref="AX3:AX8"/>
     <mergeCell ref="AX9:AX14"/>
     <mergeCell ref="AX15:AX20"/>
     <mergeCell ref="AY3:AZ8"/>
     <mergeCell ref="BA3:BB8"/>
-    <mergeCell ref="BC3:BD8"/>
-    <mergeCell ref="AY33:AZ38"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="AY9:AZ14"/>
-    <mergeCell ref="AY15:AZ20"/>
-    <mergeCell ref="AY21:AZ26"/>
-    <mergeCell ref="AY27:AZ32"/>
-    <mergeCell ref="BA9:BB14"/>
-    <mergeCell ref="BA15:BB20"/>
-    <mergeCell ref="BA21:BB26"/>
-    <mergeCell ref="BA27:BB32"/>
-    <mergeCell ref="BE27:BF32"/>
-    <mergeCell ref="BA33:BB38"/>
-    <mergeCell ref="BC33:BD38"/>
-    <mergeCell ref="BE33:BF38"/>
-    <mergeCell ref="BE3:BF8"/>
-    <mergeCell ref="BC9:BD14"/>
-    <mergeCell ref="BE9:BF14"/>
-    <mergeCell ref="BC15:BD20"/>
-    <mergeCell ref="BE15:BF20"/>
-    <mergeCell ref="BC21:BD26"/>
-    <mergeCell ref="BE21:BF26"/>
-    <mergeCell ref="BC27:BD32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new table to report
</commit_message>
<xml_diff>
--- a/Report/Empirical Data.xlsx
+++ b/Report/Empirical Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kharp\Desktop\School\2024\S2024\CSCI2226-DatastructuresAndAlgorithms\SortingProject\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3237D3DD-9C91-435E-A8FB-C488AD8973B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF31FF3-893C-4EBF-928F-384C6128AF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="79">
   <si>
     <t>Algorithm</t>
   </si>
@@ -280,9 +280,6 @@
     <t>bubble/selection</t>
   </si>
   <si>
-    <t>shellsort/selection</t>
-  </si>
-  <si>
     <t>quick/selection</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
   </si>
   <si>
     <t>insertion/selection</t>
-  </si>
-  <si>
-    <t>seslection/insesrtion</t>
   </si>
   <si>
     <t>bubble/insertion</t>
@@ -346,23 +340,33 @@
     <t>selection/shell</t>
   </si>
   <si>
-    <t>shellsort/bubble</t>
-  </si>
-  <si>
     <t>shell/log2(n) ~ insertion</t>
   </si>
   <si>
-    <t>if x/y &gt; 1 = n, then y is n times faster than x                    otherwise, x is 1/n times faster than  y</t>
+    <t>shell/bubble</t>
+  </si>
+  <si>
+    <t>shell/selection</t>
+  </si>
+  <si>
+    <t>selection/insertion</t>
+  </si>
+  <si>
+    <t>Key:                                                                          if x/y &gt; 1 = s, then y is s times faster than x                    otherwise, x is 1/s times faster than y</t>
+  </si>
+  <si>
+    <t>Key: if x/y &gt; 1 = s, then y is s times faster than x, otherwise, x is 1/s times faster than y.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -440,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +466,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,48 +847,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,15 +904,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -922,29 +929,110 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14137,10 +14225,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BI91"/>
+  <dimension ref="A1:BQ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S30" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AU39" sqref="AC2:AU39"/>
+    <sheetView tabSelected="1" topLeftCell="AN30" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BL40" sqref="BL40:BQ76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14160,100 +14248,105 @@
     <col min="37" max="37" width="8.90625" customWidth="1"/>
     <col min="41" max="41" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="AY1" s="50" t="s">
+      <c r="AY1" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="AZ1" s="51"/>
-      <c r="BA1" s="51"/>
-      <c r="BB1" s="51"/>
-      <c r="BC1" s="51"/>
-      <c r="BD1" s="52"/>
-      <c r="BE1" s="34" t="s">
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="43"/>
+      <c r="BE1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="BF1" s="35"/>
-      <c r="BG1" s="34" t="s">
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" s="35"/>
+      <c r="BH1" s="32"/>
       <c r="BI1" s="47" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="50" t="s">
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="50" t="s">
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="52"/>
-      <c r="AD2" s="50" t="s">
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="43"/>
+      <c r="AD2" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="50" t="s">
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="43"/>
+      <c r="AJ2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="50" t="s">
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
+      <c r="AO2" s="43"/>
+      <c r="AP2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="52"/>
+      <c r="AQ2" s="45"/>
+      <c r="AR2" s="45"/>
+      <c r="AS2" s="45"/>
+      <c r="AT2" s="45"/>
+      <c r="AU2" s="43"/>
       <c r="AX2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AY2" s="63" t="s">
+      <c r="AY2" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="AZ2" s="64"/>
-      <c r="BA2" s="50" t="s">
+      <c r="AZ2" s="41"/>
+      <c r="BA2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="BB2" s="52"/>
-      <c r="BC2" s="64" t="s">
+      <c r="BB2" s="43"/>
+      <c r="BC2" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="BD2" s="65"/>
-      <c r="BE2" s="38"/>
-      <c r="BF2" s="39"/>
-      <c r="BG2" s="38"/>
-      <c r="BH2" s="39"/>
+      <c r="BD2" s="44"/>
+      <c r="BE2" s="39"/>
+      <c r="BF2" s="36"/>
+      <c r="BG2" s="39"/>
+      <c r="BH2" s="36"/>
       <c r="BI2" s="48"/>
     </row>
     <row r="3" spans="1:61" ht="17" thickBot="1" x14ac:dyDescent="0.4">
@@ -14395,38 +14488,38 @@
       <c r="AU3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AX3" s="34" t="s">
+      <c r="AX3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="AY3" s="61" t="s">
+      <c r="AY3" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="AZ3" s="35"/>
-      <c r="BA3" s="62" t="s">
+      <c r="AZ3" s="32"/>
+      <c r="BA3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BB3" s="35"/>
-      <c r="BC3" s="62" t="s">
+      <c r="BB3" s="32"/>
+      <c r="BC3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BD3" s="35"/>
-      <c r="BE3" s="66" t="s">
+      <c r="BD3" s="32"/>
+      <c r="BE3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="BF3" s="35"/>
-      <c r="BG3" s="34" t="s">
+      <c r="BF3" s="32"/>
+      <c r="BG3" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="BH3" s="35"/>
+      <c r="BH3" s="32"/>
       <c r="BI3" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="10">
@@ -14567,22 +14660,22 @@
         <f>AVERAGE(AP4:AT4)</f>
         <v>2.1795882600000001</v>
       </c>
-      <c r="AX4" s="36"/>
-      <c r="AY4" s="36"/>
-      <c r="AZ4" s="37"/>
-      <c r="BA4" s="36"/>
-      <c r="BB4" s="37"/>
-      <c r="BC4" s="36"/>
-      <c r="BD4" s="37"/>
-      <c r="BE4" s="67"/>
-      <c r="BF4" s="37"/>
-      <c r="BG4" s="36"/>
-      <c r="BH4" s="37"/>
+      <c r="AX4" s="38"/>
+      <c r="AY4" s="38"/>
+      <c r="AZ4" s="34"/>
+      <c r="BA4" s="38"/>
+      <c r="BB4" s="34"/>
+      <c r="BC4" s="38"/>
+      <c r="BD4" s="34"/>
+      <c r="BE4" s="33"/>
+      <c r="BF4" s="34"/>
+      <c r="BG4" s="38"/>
+      <c r="BH4" s="34"/>
       <c r="BI4" s="48"/>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A5" s="57"/>
-      <c r="B5" s="54"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="5">
         <v>100000</v>
       </c>
@@ -14703,7 +14796,7 @@
         <v>3.9356388999999998</v>
       </c>
       <c r="AO5" s="19">
-        <f t="shared" ref="AO5:AO39" si="4">AVERAGE(AJ5:AN5)</f>
+        <f>AVERAGE(AJ5:AN5)</f>
         <v>3.7816324800000003</v>
       </c>
       <c r="AP5" s="20">
@@ -14722,25 +14815,25 @@
         <v>8.8558328999999993</v>
       </c>
       <c r="AU5" s="19">
-        <f t="shared" ref="AU5:AU39" si="5">AVERAGE(AP5:AT5)</f>
+        <f t="shared" ref="AU5:AU39" si="4">AVERAGE(AP5:AT5)</f>
         <v>8.7173875799999987</v>
       </c>
-      <c r="AX5" s="36"/>
-      <c r="AY5" s="36"/>
-      <c r="AZ5" s="37"/>
-      <c r="BA5" s="36"/>
-      <c r="BB5" s="37"/>
-      <c r="BC5" s="36"/>
-      <c r="BD5" s="37"/>
-      <c r="BE5" s="67"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="36"/>
-      <c r="BH5" s="37"/>
+      <c r="AX5" s="38"/>
+      <c r="AY5" s="38"/>
+      <c r="AZ5" s="34"/>
+      <c r="BA5" s="38"/>
+      <c r="BB5" s="34"/>
+      <c r="BC5" s="38"/>
+      <c r="BD5" s="34"/>
+      <c r="BE5" s="33"/>
+      <c r="BF5" s="34"/>
+      <c r="BG5" s="38"/>
+      <c r="BH5" s="34"/>
       <c r="BI5" s="48"/>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A6" s="57"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="5">
         <v>175000</v>
       </c>
@@ -14749,11 +14842,11 @@
         <v>1.75</v>
       </c>
       <c r="E6" s="11">
-        <f t="shared" ref="E6:E15" si="6">D6^2</f>
+        <f t="shared" ref="E6:E15" si="5">D6^2</f>
         <v>3.0625</v>
       </c>
       <c r="F6" s="11">
-        <f t="shared" ref="F6:F15" si="7">D6*LOG(D6,2)</f>
+        <f t="shared" ref="F6:F15" si="6">D6*LOG(D6,2)</f>
         <v>1.4128711136008072</v>
       </c>
       <c r="G6" s="17">
@@ -14776,7 +14869,7 @@
         <v>49.444212519999994</v>
       </c>
       <c r="M6" s="20">
-        <f t="shared" ref="M6:M9" si="8">L6/L5</f>
+        <f t="shared" ref="M6:M9" si="7">L6/L5</f>
         <v>3.0156113155003781</v>
       </c>
       <c r="N6" s="20">
@@ -14799,7 +14892,7 @@
         <v>11.52258582</v>
       </c>
       <c r="T6" s="20">
-        <f t="shared" ref="T6:T9" si="9">S6/S5</f>
+        <f t="shared" ref="T6:T9" si="8">S6/S5</f>
         <v>3.046987215426074</v>
       </c>
       <c r="U6" s="20">
@@ -14822,7 +14915,7 @@
         <v>26.446548279999995</v>
       </c>
       <c r="AA6" s="20">
-        <f t="shared" ref="AA6:AA9" si="10">Z6/Z5</f>
+        <f t="shared" ref="AA6:AA9" si="9">Z6/Z5</f>
         <v>3.0337699267467926</v>
       </c>
       <c r="AC6" s="48"/>
@@ -14861,7 +14954,7 @@
         <v>11.718612800000001</v>
       </c>
       <c r="AO6" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ6:AN6)</f>
         <v>11.52258582</v>
       </c>
       <c r="AP6" s="20">
@@ -14880,25 +14973,25 @@
         <v>26.7329179</v>
       </c>
       <c r="AU6" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>26.446548279999995</v>
       </c>
-      <c r="AX6" s="36"/>
-      <c r="AY6" s="36"/>
-      <c r="AZ6" s="37"/>
-      <c r="BA6" s="36"/>
-      <c r="BB6" s="37"/>
-      <c r="BC6" s="36"/>
-      <c r="BD6" s="37"/>
-      <c r="BE6" s="67"/>
-      <c r="BF6" s="37"/>
-      <c r="BG6" s="36"/>
-      <c r="BH6" s="37"/>
+      <c r="AX6" s="38"/>
+      <c r="AY6" s="38"/>
+      <c r="AZ6" s="34"/>
+      <c r="BA6" s="38"/>
+      <c r="BB6" s="34"/>
+      <c r="BC6" s="38"/>
+      <c r="BD6" s="34"/>
+      <c r="BE6" s="33"/>
+      <c r="BF6" s="34"/>
+      <c r="BG6" s="38"/>
+      <c r="BH6" s="34"/>
       <c r="BI6" s="48"/>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A7" s="57"/>
-      <c r="B7" s="54"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="5">
         <v>300000</v>
       </c>
@@ -14907,11 +15000,11 @@
         <v>1.7142857142857142</v>
       </c>
       <c r="E7" s="11">
+        <f t="shared" si="5"/>
+        <v>2.9387755102040813</v>
+      </c>
+      <c r="F7" s="11">
         <f t="shared" si="6"/>
-        <v>2.9387755102040813</v>
-      </c>
-      <c r="F7" s="11">
-        <f t="shared" si="7"/>
         <v>1.3330415634232318</v>
       </c>
       <c r="G7" s="17">
@@ -14934,7 +15027,7 @@
         <v>150.84097609999998</v>
       </c>
       <c r="M7" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.0507306803396936</v>
       </c>
       <c r="N7" s="20">
@@ -14957,7 +15050,7 @@
         <v>34.178462160000002</v>
       </c>
       <c r="T7" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>2.966214588801388</v>
       </c>
       <c r="U7" s="20">
@@ -14980,7 +15073,7 @@
         <v>81.228794319999992</v>
       </c>
       <c r="AA7" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>3.0714327427533772</v>
       </c>
       <c r="AC7" s="48"/>
@@ -15019,7 +15112,7 @@
         <v>34.383432499999998</v>
       </c>
       <c r="AO7" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ7:AN7)</f>
         <v>34.178462160000002</v>
       </c>
       <c r="AP7" s="20">
@@ -15038,25 +15131,25 @@
         <v>80.685685699999993</v>
       </c>
       <c r="AU7" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>81.228794319999992</v>
       </c>
-      <c r="AX7" s="36"/>
-      <c r="AY7" s="36"/>
-      <c r="AZ7" s="37"/>
-      <c r="BA7" s="36"/>
-      <c r="BB7" s="37"/>
-      <c r="BC7" s="36"/>
-      <c r="BD7" s="37"/>
-      <c r="BE7" s="67"/>
-      <c r="BF7" s="37"/>
-      <c r="BG7" s="36"/>
-      <c r="BH7" s="37"/>
+      <c r="AX7" s="38"/>
+      <c r="AY7" s="38"/>
+      <c r="AZ7" s="34"/>
+      <c r="BA7" s="38"/>
+      <c r="BB7" s="34"/>
+      <c r="BC7" s="38"/>
+      <c r="BD7" s="34"/>
+      <c r="BE7" s="33"/>
+      <c r="BF7" s="34"/>
+      <c r="BG7" s="38"/>
+      <c r="BH7" s="34"/>
       <c r="BI7" s="48"/>
     </row>
     <row r="8" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="57"/>
-      <c r="B8" s="54"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="5">
         <v>425000</v>
       </c>
@@ -15065,11 +15158,11 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="E8" s="11">
+        <f t="shared" si="5"/>
+        <v>2.0069444444444446</v>
+      </c>
+      <c r="F8" s="11">
         <f t="shared" si="6"/>
-        <v>2.0069444444444446</v>
-      </c>
-      <c r="F8" s="11">
-        <f t="shared" si="7"/>
         <v>0.71187548241634313</v>
       </c>
       <c r="G8" s="17">
@@ -15092,7 +15185,7 @@
         <v>307.67407392000001</v>
       </c>
       <c r="M8" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.0397247609696425</v>
       </c>
       <c r="N8" s="20">
@@ -15115,7 +15208,7 @@
         <v>68.704380760000006</v>
       </c>
       <c r="T8" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>2.0101659471503854</v>
       </c>
       <c r="U8" s="20">
@@ -15138,7 +15231,7 @@
         <v>159.48612682000001</v>
       </c>
       <c r="AA8" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.963418614730462</v>
       </c>
       <c r="AC8" s="48"/>
@@ -15177,7 +15270,7 @@
         <v>67.681019599999999</v>
       </c>
       <c r="AO8" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ8:AN8)</f>
         <v>68.704380760000006</v>
       </c>
       <c r="AP8" s="20">
@@ -15196,25 +15289,25 @@
         <v>160.46309980000001</v>
       </c>
       <c r="AU8" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>159.48612682000001</v>
       </c>
-      <c r="AX8" s="38"/>
-      <c r="AY8" s="38"/>
-      <c r="AZ8" s="39"/>
-      <c r="BA8" s="38"/>
-      <c r="BB8" s="39"/>
-      <c r="BC8" s="38"/>
-      <c r="BD8" s="39"/>
-      <c r="BE8" s="68"/>
-      <c r="BF8" s="39"/>
-      <c r="BG8" s="38"/>
-      <c r="BH8" s="39"/>
+      <c r="AX8" s="39"/>
+      <c r="AY8" s="39"/>
+      <c r="AZ8" s="36"/>
+      <c r="BA8" s="39"/>
+      <c r="BB8" s="36"/>
+      <c r="BC8" s="39"/>
+      <c r="BD8" s="36"/>
+      <c r="BE8" s="35"/>
+      <c r="BF8" s="36"/>
+      <c r="BG8" s="39"/>
+      <c r="BH8" s="36"/>
       <c r="BI8" s="49"/>
     </row>
     <row r="9" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="58"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="6">
         <v>550000</v>
       </c>
@@ -15223,11 +15316,11 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="E9" s="11">
+        <f t="shared" si="5"/>
+        <v>1.6747404844290659</v>
+      </c>
+      <c r="F9" s="11">
         <f t="shared" si="6"/>
-        <v>1.6747404844290659</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="7"/>
         <v>0.48137135897135735</v>
       </c>
       <c r="G9" s="22">
@@ -15250,7 +15343,7 @@
         <v>494.67564397999996</v>
       </c>
       <c r="M9" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.6077911202509161</v>
       </c>
       <c r="N9" s="25">
@@ -15273,7 +15366,7 @@
         <v>116.41577226</v>
       </c>
       <c r="T9" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1.6944446769219377</v>
       </c>
       <c r="U9" s="26">
@@ -15296,7 +15389,7 @@
         <v>262.80399759999995</v>
       </c>
       <c r="AA9" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.6478172919492053</v>
       </c>
       <c r="AC9" s="49"/>
@@ -15335,7 +15428,7 @@
         <v>116.91454210000001</v>
       </c>
       <c r="AO9" s="24">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ9:AN9)</f>
         <v>116.41577226</v>
       </c>
       <c r="AP9" s="26">
@@ -15354,41 +15447,41 @@
         <v>260.890017</v>
       </c>
       <c r="AU9" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>262.80399759999995</v>
       </c>
-      <c r="AX9" s="36" t="s">
+      <c r="AX9" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AY9" s="62" t="s">
+      <c r="AY9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="AZ9" s="35"/>
-      <c r="BA9" s="62" t="s">
+      <c r="AZ9" s="32"/>
+      <c r="BA9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BB9" s="35"/>
-      <c r="BC9" s="62" t="s">
+      <c r="BB9" s="32"/>
+      <c r="BC9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BD9" s="35"/>
-      <c r="BE9" s="66" t="s">
+      <c r="BD9" s="32"/>
+      <c r="BE9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="BF9" s="35"/>
-      <c r="BG9" s="34" t="s">
+      <c r="BF9" s="32"/>
+      <c r="BG9" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="BH9" s="35"/>
+      <c r="BH9" s="32"/>
       <c r="BI9" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="57" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="10">
@@ -15507,7 +15600,7 @@
         <v>0.89189050000000003</v>
       </c>
       <c r="AO10" s="16">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ10:AN10)</f>
         <v>0.88176837999999991</v>
       </c>
       <c r="AP10" s="13">
@@ -15526,25 +15619,25 @@
         <v>0.88712849999999999</v>
       </c>
       <c r="AU10" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.8840920000000001</v>
       </c>
-      <c r="AX10" s="36"/>
-      <c r="AY10" s="36"/>
-      <c r="AZ10" s="37"/>
-      <c r="BA10" s="36"/>
-      <c r="BB10" s="37"/>
-      <c r="BC10" s="36"/>
-      <c r="BD10" s="37"/>
-      <c r="BE10" s="67"/>
-      <c r="BF10" s="37"/>
-      <c r="BG10" s="36"/>
-      <c r="BH10" s="37"/>
+      <c r="AX10" s="38"/>
+      <c r="AY10" s="38"/>
+      <c r="AZ10" s="34"/>
+      <c r="BA10" s="38"/>
+      <c r="BB10" s="34"/>
+      <c r="BC10" s="38"/>
+      <c r="BD10" s="34"/>
+      <c r="BE10" s="33"/>
+      <c r="BF10" s="34"/>
+      <c r="BG10" s="38"/>
+      <c r="BH10" s="34"/>
       <c r="BI10" s="48"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="5">
         <v>100000</v>
       </c>
@@ -15665,7 +15758,7 @@
         <v>3.5381456999999998</v>
       </c>
       <c r="AO11" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ11:AN11)</f>
         <v>3.5121737799999999</v>
       </c>
       <c r="AP11" s="20">
@@ -15684,25 +15777,25 @@
         <v>3.6623644</v>
       </c>
       <c r="AU11" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.5525640000000003</v>
       </c>
-      <c r="AX11" s="36"/>
-      <c r="AY11" s="36"/>
-      <c r="AZ11" s="37"/>
-      <c r="BA11" s="36"/>
-      <c r="BB11" s="37"/>
-      <c r="BC11" s="36"/>
-      <c r="BD11" s="37"/>
-      <c r="BE11" s="67"/>
-      <c r="BF11" s="37"/>
-      <c r="BG11" s="36"/>
-      <c r="BH11" s="37"/>
+      <c r="AX11" s="38"/>
+      <c r="AY11" s="38"/>
+      <c r="AZ11" s="34"/>
+      <c r="BA11" s="38"/>
+      <c r="BB11" s="34"/>
+      <c r="BC11" s="38"/>
+      <c r="BD11" s="34"/>
+      <c r="BE11" s="33"/>
+      <c r="BF11" s="34"/>
+      <c r="BG11" s="38"/>
+      <c r="BH11" s="34"/>
       <c r="BI11" s="48"/>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A12" s="57"/>
-      <c r="B12" s="54"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="5">
         <v>175000</v>
       </c>
@@ -15711,11 +15804,11 @@
         <v>1.75</v>
       </c>
       <c r="E12" s="11">
+        <f t="shared" si="5"/>
+        <v>3.0625</v>
+      </c>
+      <c r="F12" s="11">
         <f t="shared" si="6"/>
-        <v>3.0625</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="7"/>
         <v>1.4128711136008072</v>
       </c>
       <c r="G12" s="17">
@@ -15738,7 +15831,7 @@
         <v>10.908895239999998</v>
       </c>
       <c r="M12" s="20">
-        <f t="shared" ref="M12:M15" si="11">L12/L11</f>
+        <f t="shared" ref="M12:M15" si="10">L12/L11</f>
         <v>3.1478757896132259</v>
       </c>
       <c r="N12" s="20">
@@ -15761,7 +15854,7 @@
         <v>11.215094599999999</v>
       </c>
       <c r="T12" s="20">
-        <f t="shared" ref="T12:T15" si="12">S12/S11</f>
+        <f t="shared" ref="T12:T15" si="11">S12/S11</f>
         <v>3.1932060605497714</v>
       </c>
       <c r="U12" s="20">
@@ -15784,7 +15877,7 @@
         <v>10.935985580000001</v>
       </c>
       <c r="AA12" s="20">
-        <f t="shared" ref="AA12:AA15" si="13">Z12/Z11</f>
+        <f t="shared" ref="AA12:AA15" si="12">Z12/Z11</f>
         <v>3.0783359793095917</v>
       </c>
       <c r="AC12" s="48"/>
@@ -15823,7 +15916,7 @@
         <v>11.1866425</v>
       </c>
       <c r="AO12" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ12:AN12)</f>
         <v>11.215094599999999</v>
       </c>
       <c r="AP12" s="20">
@@ -15842,25 +15935,25 @@
         <v>10.881433400000001</v>
       </c>
       <c r="AU12" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>10.935985580000001</v>
       </c>
-      <c r="AX12" s="36"/>
-      <c r="AY12" s="36"/>
-      <c r="AZ12" s="37"/>
-      <c r="BA12" s="36"/>
-      <c r="BB12" s="37"/>
-      <c r="BC12" s="36"/>
-      <c r="BD12" s="37"/>
-      <c r="BE12" s="67"/>
-      <c r="BF12" s="37"/>
-      <c r="BG12" s="36"/>
-      <c r="BH12" s="37"/>
+      <c r="AX12" s="38"/>
+      <c r="AY12" s="38"/>
+      <c r="AZ12" s="34"/>
+      <c r="BA12" s="38"/>
+      <c r="BB12" s="34"/>
+      <c r="BC12" s="38"/>
+      <c r="BD12" s="34"/>
+      <c r="BE12" s="33"/>
+      <c r="BF12" s="34"/>
+      <c r="BG12" s="38"/>
+      <c r="BH12" s="34"/>
       <c r="BI12" s="48"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A13" s="57"/>
-      <c r="B13" s="54"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="5">
         <v>300000</v>
       </c>
@@ -15869,11 +15962,11 @@
         <v>1.7142857142857142</v>
       </c>
       <c r="E13" s="11">
+        <f t="shared" si="5"/>
+        <v>2.9387755102040813</v>
+      </c>
+      <c r="F13" s="11">
         <f t="shared" si="6"/>
-        <v>2.9387755102040813</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="7"/>
         <v>1.3330415634232318</v>
       </c>
       <c r="G13" s="17">
@@ -15896,7 +15989,7 @@
         <v>31.52791706</v>
       </c>
       <c r="M13" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2.8901109018258393</v>
       </c>
       <c r="N13" s="20">
@@ -15919,7 +16012,7 @@
         <v>32.676205999999993</v>
       </c>
       <c r="T13" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.9135916517369367</v>
       </c>
       <c r="U13" s="20">
@@ -15942,7 +16035,7 @@
         <v>32.4724115</v>
       </c>
       <c r="AA13" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>2.96931732969604</v>
       </c>
       <c r="AC13" s="48"/>
@@ -15981,7 +16074,7 @@
         <v>32.084002900000002</v>
       </c>
       <c r="AO13" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ13:AN13)</f>
         <v>32.676205999999993</v>
       </c>
       <c r="AP13" s="20">
@@ -16000,25 +16093,25 @@
         <v>32.730861500000003</v>
       </c>
       <c r="AU13" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>32.4724115</v>
       </c>
-      <c r="AX13" s="36"/>
-      <c r="AY13" s="36"/>
-      <c r="AZ13" s="37"/>
-      <c r="BA13" s="36"/>
-      <c r="BB13" s="37"/>
-      <c r="BC13" s="36"/>
-      <c r="BD13" s="37"/>
-      <c r="BE13" s="67"/>
-      <c r="BF13" s="37"/>
-      <c r="BG13" s="36"/>
-      <c r="BH13" s="37"/>
+      <c r="AX13" s="38"/>
+      <c r="AY13" s="38"/>
+      <c r="AZ13" s="34"/>
+      <c r="BA13" s="38"/>
+      <c r="BB13" s="34"/>
+      <c r="BC13" s="38"/>
+      <c r="BD13" s="34"/>
+      <c r="BE13" s="33"/>
+      <c r="BF13" s="34"/>
+      <c r="BG13" s="38"/>
+      <c r="BH13" s="34"/>
       <c r="BI13" s="48"/>
     </row>
     <row r="14" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="57"/>
-      <c r="B14" s="54"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="5">
         <v>425000</v>
       </c>
@@ -16027,11 +16120,11 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="E14" s="11">
+        <f t="shared" si="5"/>
+        <v>2.0069444444444446</v>
+      </c>
+      <c r="F14" s="11">
         <f t="shared" si="6"/>
-        <v>2.0069444444444446</v>
-      </c>
-      <c r="F14" s="11">
-        <f t="shared" si="7"/>
         <v>0.71187548241634313</v>
       </c>
       <c r="G14" s="17">
@@ -16054,7 +16147,7 @@
         <v>66.703100739999996</v>
       </c>
       <c r="M14" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2.1156837165315734</v>
       </c>
       <c r="N14" s="20">
@@ -16077,7 +16170,7 @@
         <v>66.039244200000013</v>
       </c>
       <c r="T14" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.0210193374347081</v>
       </c>
       <c r="U14" s="20">
@@ -16100,7 +16193,7 @@
         <v>64.411971059999999</v>
       </c>
       <c r="AA14" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.9835906261535272</v>
       </c>
       <c r="AC14" s="48"/>
@@ -16139,7 +16232,7 @@
         <v>64.619699600000004</v>
       </c>
       <c r="AO14" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ14:AN14)</f>
         <v>66.039244200000013</v>
       </c>
       <c r="AP14" s="20">
@@ -16158,25 +16251,25 @@
         <v>64.699296700000005</v>
       </c>
       <c r="AU14" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>64.411971059999999</v>
       </c>
-      <c r="AX14" s="38"/>
-      <c r="AY14" s="38"/>
-      <c r="AZ14" s="39"/>
-      <c r="BA14" s="38"/>
-      <c r="BB14" s="39"/>
-      <c r="BC14" s="38"/>
-      <c r="BD14" s="39"/>
-      <c r="BE14" s="68"/>
-      <c r="BF14" s="39"/>
-      <c r="BG14" s="38"/>
-      <c r="BH14" s="39"/>
+      <c r="AX14" s="39"/>
+      <c r="AY14" s="39"/>
+      <c r="AZ14" s="36"/>
+      <c r="BA14" s="39"/>
+      <c r="BB14" s="36"/>
+      <c r="BC14" s="39"/>
+      <c r="BD14" s="36"/>
+      <c r="BE14" s="35"/>
+      <c r="BF14" s="36"/>
+      <c r="BG14" s="39"/>
+      <c r="BH14" s="36"/>
       <c r="BI14" s="49"/>
     </row>
     <row r="15" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="58"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="6">
         <v>550000</v>
       </c>
@@ -16185,11 +16278,11 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="E15" s="11">
+        <f t="shared" si="5"/>
+        <v>1.6747404844290659</v>
+      </c>
+      <c r="F15" s="11">
         <f t="shared" si="6"/>
-        <v>1.6747404844290659</v>
-      </c>
-      <c r="F15" s="11">
-        <f t="shared" si="7"/>
         <v>0.48137135897135735</v>
       </c>
       <c r="G15" s="22">
@@ -16212,7 +16305,7 @@
         <v>109.7235924</v>
       </c>
       <c r="M15" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.6449548998882118</v>
       </c>
       <c r="N15" s="25">
@@ -16235,7 +16328,7 @@
         <v>110.81666572000002</v>
       </c>
       <c r="T15" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1.6780426103059489</v>
       </c>
       <c r="U15" s="25">
@@ -16258,7 +16351,7 @@
         <v>110.83381118</v>
       </c>
       <c r="AA15" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.7207020582673658</v>
       </c>
       <c r="AC15" s="49"/>
@@ -16297,7 +16390,7 @@
         <v>109.3390679</v>
       </c>
       <c r="AO15" s="24">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ15:AN15)</f>
         <v>110.81666572000002</v>
       </c>
       <c r="AP15" s="25">
@@ -16316,41 +16409,41 @@
         <v>113.26993659999999</v>
       </c>
       <c r="AU15" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>110.83381118</v>
       </c>
-      <c r="AX15" s="34" t="s">
+      <c r="AX15" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="AY15" s="62" t="s">
+      <c r="AY15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AZ15" s="35"/>
-      <c r="BA15" s="62" t="s">
+      <c r="AZ15" s="32"/>
+      <c r="BA15" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BB15" s="35"/>
-      <c r="BC15" s="62" t="s">
+      <c r="BB15" s="32"/>
+      <c r="BC15" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BD15" s="35"/>
-      <c r="BE15" s="66" t="s">
+      <c r="BD15" s="32"/>
+      <c r="BE15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="BF15" s="35"/>
-      <c r="BG15" s="34" t="s">
+      <c r="BF15" s="32"/>
+      <c r="BG15" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="BH15" s="35"/>
+      <c r="BH15" s="32"/>
       <c r="BI15" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="57" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="10">
@@ -16469,7 +16562,7 @@
         <v>8.6700000000000007E-5</v>
       </c>
       <c r="AO16" s="16">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ16:AN16)</f>
         <v>9.8480000000000006E-5</v>
       </c>
       <c r="AP16" s="20">
@@ -16488,25 +16581,25 @@
         <v>1.1501872</v>
       </c>
       <c r="AU16" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1173522599999999</v>
       </c>
-      <c r="AX16" s="36"/>
-      <c r="AY16" s="36"/>
-      <c r="AZ16" s="37"/>
-      <c r="BA16" s="36"/>
-      <c r="BB16" s="37"/>
-      <c r="BC16" s="36"/>
-      <c r="BD16" s="37"/>
-      <c r="BE16" s="67"/>
-      <c r="BF16" s="37"/>
-      <c r="BG16" s="36"/>
-      <c r="BH16" s="37"/>
+      <c r="AX16" s="38"/>
+      <c r="AY16" s="38"/>
+      <c r="AZ16" s="34"/>
+      <c r="BA16" s="38"/>
+      <c r="BB16" s="34"/>
+      <c r="BC16" s="38"/>
+      <c r="BD16" s="34"/>
+      <c r="BE16" s="33"/>
+      <c r="BF16" s="34"/>
+      <c r="BG16" s="38"/>
+      <c r="BH16" s="34"/>
       <c r="BI16" s="48"/>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A17" s="57"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="5">
         <v>100000</v>
       </c>
@@ -16627,7 +16720,7 @@
         <v>1.6809999999999999E-4</v>
       </c>
       <c r="AO17" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ17:AN17)</f>
         <v>1.4724000000000001E-4</v>
       </c>
       <c r="AP17" s="20">
@@ -16646,25 +16739,25 @@
         <v>4.4334512999999998</v>
       </c>
       <c r="AU17" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.3320717799999997</v>
       </c>
-      <c r="AX17" s="36"/>
-      <c r="AY17" s="36"/>
-      <c r="AZ17" s="37"/>
-      <c r="BA17" s="36"/>
-      <c r="BB17" s="37"/>
-      <c r="BC17" s="36"/>
-      <c r="BD17" s="37"/>
-      <c r="BE17" s="67"/>
-      <c r="BF17" s="37"/>
-      <c r="BG17" s="36"/>
-      <c r="BH17" s="37"/>
+      <c r="AX17" s="38"/>
+      <c r="AY17" s="38"/>
+      <c r="AZ17" s="34"/>
+      <c r="BA17" s="38"/>
+      <c r="BB17" s="34"/>
+      <c r="BC17" s="38"/>
+      <c r="BD17" s="34"/>
+      <c r="BE17" s="33"/>
+      <c r="BF17" s="34"/>
+      <c r="BG17" s="38"/>
+      <c r="BH17" s="34"/>
       <c r="BI17" s="48"/>
     </row>
     <row r="18" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A18" s="57"/>
-      <c r="B18" s="54"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="5">
         <v>175000</v>
       </c>
@@ -16673,11 +16766,11 @@
         <v>1.75</v>
       </c>
       <c r="E18" s="11">
-        <f t="shared" ref="E18:E21" si="14">D18^2</f>
+        <f t="shared" ref="E18:E21" si="13">D18^2</f>
         <v>3.0625</v>
       </c>
       <c r="F18" s="11">
-        <f t="shared" ref="F18:F21" si="15">D18*LOG(D18,2)</f>
+        <f t="shared" ref="F18:F21" si="14">D18*LOG(D18,2)</f>
         <v>1.4128711136008072</v>
       </c>
       <c r="G18" s="17">
@@ -16700,7 +16793,7 @@
         <v>6.8691384599999994</v>
       </c>
       <c r="M18" s="20">
-        <f t="shared" ref="M18:M21" si="16">L18/L17</f>
+        <f t="shared" ref="M18:M21" si="15">L18/L17</f>
         <v>3.1027733265740101</v>
       </c>
       <c r="N18" s="20">
@@ -16723,7 +16816,7 @@
         <v>2.6708E-4</v>
       </c>
       <c r="T18" s="20">
-        <f t="shared" ref="T18:T21" si="17">S18/S17</f>
+        <f t="shared" ref="T18:T21" si="16">S18/S17</f>
         <v>1.8139092637870142</v>
       </c>
       <c r="U18" s="20">
@@ -16746,7 +16839,7 @@
         <v>13.35462506</v>
       </c>
       <c r="AA18" s="20">
-        <f t="shared" ref="AA18:AA21" si="18">Z18/Z17</f>
+        <f t="shared" ref="AA18:AA21" si="17">Z18/Z17</f>
         <v>3.0827340215493848</v>
       </c>
       <c r="AC18" s="48"/>
@@ -16785,7 +16878,7 @@
         <v>3.8690000000000003E-4</v>
       </c>
       <c r="AO18" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ18:AN18)</f>
         <v>2.6708E-4</v>
       </c>
       <c r="AP18" s="20">
@@ -16804,25 +16897,25 @@
         <v>13.5598308</v>
       </c>
       <c r="AU18" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>13.35462506</v>
       </c>
-      <c r="AX18" s="36"/>
-      <c r="AY18" s="36"/>
-      <c r="AZ18" s="37"/>
-      <c r="BA18" s="36"/>
-      <c r="BB18" s="37"/>
-      <c r="BC18" s="36"/>
-      <c r="BD18" s="37"/>
-      <c r="BE18" s="67"/>
-      <c r="BF18" s="37"/>
-      <c r="BG18" s="36"/>
-      <c r="BH18" s="37"/>
+      <c r="AX18" s="38"/>
+      <c r="AY18" s="38"/>
+      <c r="AZ18" s="34"/>
+      <c r="BA18" s="38"/>
+      <c r="BB18" s="34"/>
+      <c r="BC18" s="38"/>
+      <c r="BD18" s="34"/>
+      <c r="BE18" s="33"/>
+      <c r="BF18" s="34"/>
+      <c r="BG18" s="38"/>
+      <c r="BH18" s="34"/>
       <c r="BI18" s="48"/>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A19" s="57"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="5">
         <v>300000</v>
       </c>
@@ -16831,11 +16924,11 @@
         <v>1.7142857142857142</v>
       </c>
       <c r="E19" s="11">
+        <f t="shared" si="13"/>
+        <v>2.9387755102040813</v>
+      </c>
+      <c r="F19" s="11">
         <f t="shared" si="14"/>
-        <v>2.9387755102040813</v>
-      </c>
-      <c r="F19" s="11">
-        <f t="shared" si="15"/>
         <v>1.3330415634232318</v>
       </c>
       <c r="G19" s="17">
@@ -16858,7 +16951,7 @@
         <v>20.141167800000002</v>
       </c>
       <c r="M19" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2.9321243001993591</v>
       </c>
       <c r="N19" s="20">
@@ -16881,7 +16974,7 @@
         <v>5.2304000000000001E-4</v>
       </c>
       <c r="T19" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1.9583645349707952</v>
       </c>
       <c r="U19" s="20">
@@ -16904,7 +16997,7 @@
         <v>41.141370479999999</v>
       </c>
       <c r="AA19" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>3.0806833059826841</v>
       </c>
       <c r="AC19" s="48"/>
@@ -16943,7 +17036,7 @@
         <v>4.2949999999999998E-4</v>
       </c>
       <c r="AO19" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ19:AN19)</f>
         <v>5.2304000000000001E-4</v>
       </c>
       <c r="AP19" s="20">
@@ -16962,25 +17055,25 @@
         <v>41.462623999999998</v>
       </c>
       <c r="AU19" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>41.141370479999999</v>
       </c>
-      <c r="AX19" s="36"/>
-      <c r="AY19" s="36"/>
-      <c r="AZ19" s="37"/>
-      <c r="BA19" s="36"/>
-      <c r="BB19" s="37"/>
-      <c r="BC19" s="36"/>
-      <c r="BD19" s="37"/>
-      <c r="BE19" s="67"/>
-      <c r="BF19" s="37"/>
-      <c r="BG19" s="36"/>
-      <c r="BH19" s="37"/>
+      <c r="AX19" s="38"/>
+      <c r="AY19" s="38"/>
+      <c r="AZ19" s="34"/>
+      <c r="BA19" s="38"/>
+      <c r="BB19" s="34"/>
+      <c r="BC19" s="38"/>
+      <c r="BD19" s="34"/>
+      <c r="BE19" s="33"/>
+      <c r="BF19" s="34"/>
+      <c r="BG19" s="38"/>
+      <c r="BH19" s="34"/>
       <c r="BI19" s="48"/>
     </row>
     <row r="20" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="57"/>
-      <c r="B20" s="54"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="5">
         <v>425000</v>
       </c>
@@ -16989,11 +17082,11 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="E20" s="11">
+        <f t="shared" si="13"/>
+        <v>2.0069444444444446</v>
+      </c>
+      <c r="F20" s="11">
         <f t="shared" si="14"/>
-        <v>2.0069444444444446</v>
-      </c>
-      <c r="F20" s="11">
-        <f t="shared" si="15"/>
         <v>0.71187548241634313</v>
       </c>
       <c r="G20" s="17">
@@ -17016,7 +17109,7 @@
         <v>40.321519960000003</v>
       </c>
       <c r="M20" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2.0019454860010648</v>
       </c>
       <c r="N20" s="18">
@@ -17039,7 +17132,7 @@
         <v>6.4141999999999997E-4</v>
       </c>
       <c r="T20" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1.2263306821657998</v>
       </c>
       <c r="U20" s="20">
@@ -17062,7 +17155,7 @@
         <v>82.394224699999995</v>
       </c>
       <c r="AA20" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>2.0027097721514697</v>
       </c>
       <c r="AC20" s="48"/>
@@ -17101,7 +17194,7 @@
         <v>6.0930000000000001E-4</v>
       </c>
       <c r="AO20" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ20:AN20)</f>
         <v>6.4141999999999997E-4</v>
       </c>
       <c r="AP20" s="20">
@@ -17120,25 +17213,25 @@
         <v>81.754149699999999</v>
       </c>
       <c r="AU20" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>82.394224699999995</v>
       </c>
-      <c r="AX20" s="38"/>
-      <c r="AY20" s="38"/>
-      <c r="AZ20" s="39"/>
-      <c r="BA20" s="38"/>
-      <c r="BB20" s="39"/>
-      <c r="BC20" s="38"/>
-      <c r="BD20" s="39"/>
-      <c r="BE20" s="68"/>
-      <c r="BF20" s="39"/>
-      <c r="BG20" s="38"/>
-      <c r="BH20" s="39"/>
+      <c r="AX20" s="39"/>
+      <c r="AY20" s="39"/>
+      <c r="AZ20" s="36"/>
+      <c r="BA20" s="39"/>
+      <c r="BB20" s="36"/>
+      <c r="BC20" s="39"/>
+      <c r="BD20" s="36"/>
+      <c r="BE20" s="35"/>
+      <c r="BF20" s="36"/>
+      <c r="BG20" s="39"/>
+      <c r="BH20" s="36"/>
       <c r="BI20" s="49"/>
     </row>
     <row r="21" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="58"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="6">
         <v>550000</v>
       </c>
@@ -17147,11 +17240,11 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="E21" s="11">
+        <f t="shared" si="13"/>
+        <v>1.6747404844290659</v>
+      </c>
+      <c r="F21" s="11">
         <f t="shared" si="14"/>
-        <v>1.6747404844290659</v>
-      </c>
-      <c r="F21" s="11">
-        <f t="shared" si="15"/>
         <v>0.48137135897135735</v>
       </c>
       <c r="G21" s="22">
@@ -17174,7 +17267,7 @@
         <v>66.27940498000001</v>
       </c>
       <c r="M21" s="20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1.6437724829260132</v>
       </c>
       <c r="N21" s="20">
@@ -17197,7 +17290,7 @@
         <v>8.0061999999999993E-4</v>
       </c>
       <c r="T21" s="20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1.2481993077858502</v>
       </c>
       <c r="U21" s="26">
@@ -17220,7 +17313,7 @@
         <v>135.94702348000001</v>
       </c>
       <c r="AA21" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>1.6499581612059275</v>
       </c>
       <c r="AC21" s="49"/>
@@ -17259,7 +17352,7 @@
         <v>7.6760000000000001E-4</v>
       </c>
       <c r="AO21" s="24">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ21:AN21)</f>
         <v>8.0061999999999993E-4</v>
       </c>
       <c r="AP21" s="26">
@@ -17278,41 +17371,41 @@
         <v>132.62209770000001</v>
       </c>
       <c r="AU21" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>135.94702348000001</v>
       </c>
-      <c r="AX21" s="34" t="s">
+      <c r="AX21" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AY21" s="62" t="s">
+      <c r="AY21" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="AZ21" s="35"/>
-      <c r="BA21" s="62" t="s">
+      <c r="AZ21" s="32"/>
+      <c r="BA21" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="BB21" s="35"/>
-      <c r="BC21" s="62" t="s">
+      <c r="BB21" s="32"/>
+      <c r="BC21" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="BD21" s="35"/>
-      <c r="BE21" s="66" t="s">
+      <c r="BD21" s="32"/>
+      <c r="BE21" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="BF21" s="35"/>
-      <c r="BG21" s="34" t="s">
+      <c r="BF21" s="32"/>
+      <c r="BG21" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="BH21" s="35"/>
+      <c r="BH21" s="32"/>
       <c r="BI21" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="10">
@@ -17431,7 +17524,7 @@
         <v>2.9645700000000001E-2</v>
       </c>
       <c r="AO22" s="16">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ22:AN22)</f>
         <v>3.2456680000000002E-2</v>
       </c>
       <c r="AP22" s="13">
@@ -17450,25 +17543,25 @@
         <v>2.05493E-2</v>
       </c>
       <c r="AU22" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1009380000000001E-2</v>
       </c>
-      <c r="AX22" s="36"/>
-      <c r="AY22" s="36"/>
-      <c r="AZ22" s="37"/>
-      <c r="BA22" s="36"/>
-      <c r="BB22" s="37"/>
-      <c r="BC22" s="36"/>
-      <c r="BD22" s="37"/>
-      <c r="BE22" s="67"/>
-      <c r="BF22" s="37"/>
-      <c r="BG22" s="36"/>
-      <c r="BH22" s="37"/>
+      <c r="AX22" s="38"/>
+      <c r="AY22" s="38"/>
+      <c r="AZ22" s="34"/>
+      <c r="BA22" s="38"/>
+      <c r="BB22" s="34"/>
+      <c r="BC22" s="38"/>
+      <c r="BD22" s="34"/>
+      <c r="BE22" s="33"/>
+      <c r="BF22" s="34"/>
+      <c r="BG22" s="38"/>
+      <c r="BH22" s="34"/>
       <c r="BI22" s="48"/>
     </row>
     <row r="23" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A23" s="57"/>
-      <c r="B23" s="54"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="5">
         <v>100000</v>
       </c>
@@ -17589,7 +17682,7 @@
         <v>4.6229800000000001E-2</v>
       </c>
       <c r="AO23" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ23:AN23)</f>
         <v>4.4936039999999997E-2</v>
       </c>
       <c r="AP23" s="20">
@@ -17608,25 +17701,25 @@
         <v>3.7886200000000002E-2</v>
       </c>
       <c r="AU23" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.9191080000000003E-2</v>
       </c>
-      <c r="AX23" s="36"/>
-      <c r="AY23" s="36"/>
-      <c r="AZ23" s="37"/>
-      <c r="BA23" s="36"/>
-      <c r="BB23" s="37"/>
-      <c r="BC23" s="36"/>
-      <c r="BD23" s="37"/>
-      <c r="BE23" s="67"/>
-      <c r="BF23" s="37"/>
-      <c r="BG23" s="36"/>
-      <c r="BH23" s="37"/>
+      <c r="AX23" s="38"/>
+      <c r="AY23" s="38"/>
+      <c r="AZ23" s="34"/>
+      <c r="BA23" s="38"/>
+      <c r="BB23" s="34"/>
+      <c r="BC23" s="38"/>
+      <c r="BD23" s="34"/>
+      <c r="BE23" s="33"/>
+      <c r="BF23" s="34"/>
+      <c r="BG23" s="38"/>
+      <c r="BH23" s="34"/>
       <c r="BI23" s="48"/>
     </row>
     <row r="24" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A24" s="57"/>
-      <c r="B24" s="54"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="5">
         <v>175000</v>
       </c>
@@ -17635,11 +17728,11 @@
         <v>1.75</v>
       </c>
       <c r="E24" s="11">
-        <f t="shared" ref="E24:E27" si="19">D24^2</f>
+        <f t="shared" ref="E24:E27" si="18">D24^2</f>
         <v>3.0625</v>
       </c>
       <c r="F24" s="11">
-        <f t="shared" ref="F24:F27" si="20">D24*LOG(D24,2)</f>
+        <f t="shared" ref="F24:F27" si="19">D24*LOG(D24,2)</f>
         <v>1.4128711136008072</v>
       </c>
       <c r="G24" s="17">
@@ -17662,7 +17755,7 @@
         <v>8.4175180000000002E-2</v>
       </c>
       <c r="M24" s="20">
-        <f t="shared" ref="M24:M27" si="21">L24/L23</f>
+        <f t="shared" ref="M24:M27" si="20">L24/L23</f>
         <v>1.6969762337147078</v>
       </c>
       <c r="N24" s="20">
@@ -17685,7 +17778,7 @@
         <v>7.6540840000000013E-2</v>
       </c>
       <c r="T24" s="20">
-        <f t="shared" ref="T24:T27" si="22">S24/S23</f>
+        <f t="shared" ref="T24:T27" si="21">S24/S23</f>
         <v>1.703328553205846</v>
       </c>
       <c r="U24" s="20">
@@ -17708,7 +17801,7 @@
         <v>6.838284E-2</v>
       </c>
       <c r="AA24" s="20">
-        <f t="shared" ref="AA24:AA27" si="23">Z24/Z23</f>
+        <f t="shared" ref="AA24:AA27" si="22">Z24/Z23</f>
         <v>1.7448572481289109</v>
       </c>
       <c r="AC24" s="48"/>
@@ -17747,7 +17840,7 @@
         <v>7.4467099999999994E-2</v>
       </c>
       <c r="AO24" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ24:AN24)</f>
         <v>7.6540840000000013E-2</v>
       </c>
       <c r="AP24" s="20">
@@ -17766,25 +17859,25 @@
         <v>6.6806599999999994E-2</v>
       </c>
       <c r="AU24" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.838284E-2</v>
       </c>
-      <c r="AX24" s="36"/>
-      <c r="AY24" s="36"/>
-      <c r="AZ24" s="37"/>
-      <c r="BA24" s="36"/>
-      <c r="BB24" s="37"/>
-      <c r="BC24" s="36"/>
-      <c r="BD24" s="37"/>
-      <c r="BE24" s="67"/>
-      <c r="BF24" s="37"/>
-      <c r="BG24" s="36"/>
-      <c r="BH24" s="37"/>
+      <c r="AX24" s="38"/>
+      <c r="AY24" s="38"/>
+      <c r="AZ24" s="34"/>
+      <c r="BA24" s="38"/>
+      <c r="BB24" s="34"/>
+      <c r="BC24" s="38"/>
+      <c r="BD24" s="34"/>
+      <c r="BE24" s="33"/>
+      <c r="BF24" s="34"/>
+      <c r="BG24" s="38"/>
+      <c r="BH24" s="34"/>
       <c r="BI24" s="48"/>
     </row>
     <row r="25" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A25" s="57"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="5">
         <v>300000</v>
       </c>
@@ -17793,11 +17886,11 @@
         <v>1.7142857142857142</v>
       </c>
       <c r="E25" s="11">
+        <f t="shared" si="18"/>
+        <v>2.9387755102040813</v>
+      </c>
+      <c r="F25" s="11">
         <f t="shared" si="19"/>
-        <v>2.9387755102040813</v>
-      </c>
-      <c r="F25" s="11">
-        <f t="shared" si="20"/>
         <v>1.3330415634232318</v>
       </c>
       <c r="G25" s="17">
@@ -17820,7 +17913,7 @@
         <v>0.14635941999999999</v>
       </c>
       <c r="M25" s="20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>1.738747930209356</v>
       </c>
       <c r="N25" s="20">
@@ -17843,7 +17936,7 @@
         <v>0.13504572000000001</v>
       </c>
       <c r="T25" s="20">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>1.7643616140089393</v>
       </c>
       <c r="U25" s="20">
@@ -17866,7 +17959,7 @@
         <v>0.11834768</v>
       </c>
       <c r="AA25" s="20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>1.7306634237478291</v>
       </c>
       <c r="AC25" s="48"/>
@@ -17905,7 +17998,7 @@
         <v>0.142403</v>
       </c>
       <c r="AO25" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ25:AN25)</f>
         <v>0.13504572000000001</v>
       </c>
       <c r="AP25" s="20">
@@ -17924,25 +18017,25 @@
         <v>0.1250452</v>
       </c>
       <c r="AU25" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.11834768</v>
       </c>
-      <c r="AX25" s="36"/>
-      <c r="AY25" s="36"/>
-      <c r="AZ25" s="37"/>
-      <c r="BA25" s="36"/>
-      <c r="BB25" s="37"/>
-      <c r="BC25" s="36"/>
-      <c r="BD25" s="37"/>
-      <c r="BE25" s="67"/>
-      <c r="BF25" s="37"/>
-      <c r="BG25" s="36"/>
-      <c r="BH25" s="37"/>
+      <c r="AX25" s="38"/>
+      <c r="AY25" s="38"/>
+      <c r="AZ25" s="34"/>
+      <c r="BA25" s="38"/>
+      <c r="BB25" s="34"/>
+      <c r="BC25" s="38"/>
+      <c r="BD25" s="34"/>
+      <c r="BE25" s="33"/>
+      <c r="BF25" s="34"/>
+      <c r="BG25" s="38"/>
+      <c r="BH25" s="34"/>
       <c r="BI25" s="48"/>
     </row>
     <row r="26" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="57"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="5">
         <v>425000</v>
       </c>
@@ -17951,11 +18044,11 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="E26" s="11">
+        <f t="shared" si="18"/>
+        <v>2.0069444444444446</v>
+      </c>
+      <c r="F26" s="11">
         <f t="shared" si="19"/>
-        <v>2.0069444444444446</v>
-      </c>
-      <c r="F26" s="11">
-        <f t="shared" si="20"/>
         <v>0.71187548241634313</v>
       </c>
       <c r="G26" s="17">
@@ -17978,7 +18071,7 @@
         <v>0.2058516</v>
       </c>
       <c r="M26" s="20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>1.4064800202132532</v>
       </c>
       <c r="N26" s="20">
@@ -18001,7 +18094,7 @@
         <v>0.19297686</v>
       </c>
       <c r="T26" s="20">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>1.4289742762673263</v>
       </c>
       <c r="U26" s="20">
@@ -18024,7 +18117,7 @@
         <v>0.16483602000000003</v>
       </c>
       <c r="AA26" s="20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>1.392811587012099</v>
       </c>
       <c r="AC26" s="48"/>
@@ -18063,7 +18156,7 @@
         <v>0.1899264</v>
       </c>
       <c r="AO26" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ26:AN26)</f>
         <v>0.19297686</v>
       </c>
       <c r="AP26" s="20">
@@ -18082,25 +18175,25 @@
         <v>0.15979070000000001</v>
       </c>
       <c r="AU26" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.16483602000000003</v>
       </c>
-      <c r="AX26" s="38"/>
-      <c r="AY26" s="38"/>
-      <c r="AZ26" s="39"/>
-      <c r="BA26" s="38"/>
-      <c r="BB26" s="39"/>
-      <c r="BC26" s="38"/>
-      <c r="BD26" s="39"/>
-      <c r="BE26" s="68"/>
-      <c r="BF26" s="39"/>
-      <c r="BG26" s="38"/>
-      <c r="BH26" s="39"/>
+      <c r="AX26" s="39"/>
+      <c r="AY26" s="39"/>
+      <c r="AZ26" s="36"/>
+      <c r="BA26" s="39"/>
+      <c r="BB26" s="36"/>
+      <c r="BC26" s="39"/>
+      <c r="BD26" s="36"/>
+      <c r="BE26" s="35"/>
+      <c r="BF26" s="36"/>
+      <c r="BG26" s="39"/>
+      <c r="BH26" s="36"/>
       <c r="BI26" s="49"/>
     </row>
     <row r="27" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="58"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="6">
         <v>550000</v>
       </c>
@@ -18109,11 +18202,11 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="E27" s="11">
+        <f t="shared" si="18"/>
+        <v>1.6747404844290659</v>
+      </c>
+      <c r="F27" s="11">
         <f t="shared" si="19"/>
-        <v>1.6747404844290659</v>
-      </c>
-      <c r="F27" s="11">
-        <f t="shared" si="20"/>
         <v>0.48137135897135735</v>
       </c>
       <c r="G27" s="22">
@@ -18136,7 +18229,7 @@
         <v>0.26584922</v>
       </c>
       <c r="M27" s="20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>1.291460547306895</v>
       </c>
       <c r="N27" s="25">
@@ -18159,7 +18252,7 @@
         <v>0.25202259999999999</v>
       </c>
       <c r="T27" s="20">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>1.3059731617562851</v>
       </c>
       <c r="U27" s="25">
@@ -18182,7 +18275,7 @@
         <v>0.21743744000000001</v>
       </c>
       <c r="AA27" s="20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>1.3191136257718428</v>
       </c>
       <c r="AC27" s="49"/>
@@ -18221,7 +18314,7 @@
         <v>0.2566425</v>
       </c>
       <c r="AO27" s="24">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ27:AN27)</f>
         <v>0.25202259999999999</v>
       </c>
       <c r="AP27" s="25">
@@ -18240,41 +18333,41 @@
         <v>0.2260112</v>
       </c>
       <c r="AU27" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.21743744000000001</v>
       </c>
-      <c r="AX27" s="34" t="s">
+      <c r="AX27" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="AY27" s="62" t="s">
+      <c r="AY27" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="AZ27" s="35"/>
-      <c r="BA27" s="62" t="s">
+      <c r="AZ27" s="32"/>
+      <c r="BA27" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BB27" s="35"/>
-      <c r="BC27" s="62" t="s">
+      <c r="BB27" s="32"/>
+      <c r="BC27" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="BD27" s="35"/>
-      <c r="BE27" s="66" t="s">
+      <c r="BD27" s="32"/>
+      <c r="BE27" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="BF27" s="35"/>
-      <c r="BG27" s="41" t="s">
+      <c r="BF27" s="32"/>
+      <c r="BG27" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="BH27" s="42"/>
+      <c r="BH27" s="60"/>
       <c r="BI27" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="57" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="10">
@@ -18393,7 +18486,7 @@
         <v>9.990000000000001E-4</v>
       </c>
       <c r="AO28" s="16">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ28:AN28)</f>
         <v>1.3991399999999999E-3</v>
       </c>
       <c r="AP28" s="13">
@@ -18412,25 +18505,25 @@
         <v>2.1056999999999998E-3</v>
       </c>
       <c r="AU28" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1247800000000002E-3</v>
       </c>
-      <c r="AX28" s="36"/>
-      <c r="AY28" s="36"/>
-      <c r="AZ28" s="37"/>
-      <c r="BA28" s="36"/>
-      <c r="BB28" s="37"/>
-      <c r="BC28" s="36"/>
-      <c r="BD28" s="37"/>
-      <c r="BE28" s="67"/>
-      <c r="BF28" s="37"/>
-      <c r="BG28" s="43"/>
-      <c r="BH28" s="44"/>
+      <c r="AX28" s="38"/>
+      <c r="AY28" s="38"/>
+      <c r="AZ28" s="34"/>
+      <c r="BA28" s="38"/>
+      <c r="BB28" s="34"/>
+      <c r="BC28" s="38"/>
+      <c r="BD28" s="34"/>
+      <c r="BE28" s="33"/>
+      <c r="BF28" s="34"/>
+      <c r="BG28" s="61"/>
+      <c r="BH28" s="62"/>
       <c r="BI28" s="48"/>
     </row>
     <row r="29" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A29" s="57"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="5">
         <v>100000</v>
       </c>
@@ -18551,7 +18644,7 @@
         <v>2.2461999999999998E-3</v>
       </c>
       <c r="AO29" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ29:AN29)</f>
         <v>2.2692799999999998E-3</v>
       </c>
       <c r="AP29" s="20">
@@ -18570,25 +18663,25 @@
         <v>4.1974999999999998E-3</v>
       </c>
       <c r="AU29" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.1765199999999995E-3</v>
       </c>
-      <c r="AX29" s="36"/>
-      <c r="AY29" s="36"/>
-      <c r="AZ29" s="37"/>
-      <c r="BA29" s="36"/>
-      <c r="BB29" s="37"/>
-      <c r="BC29" s="36"/>
-      <c r="BD29" s="37"/>
-      <c r="BE29" s="67"/>
-      <c r="BF29" s="37"/>
-      <c r="BG29" s="43"/>
-      <c r="BH29" s="44"/>
+      <c r="AX29" s="38"/>
+      <c r="AY29" s="38"/>
+      <c r="AZ29" s="34"/>
+      <c r="BA29" s="38"/>
+      <c r="BB29" s="34"/>
+      <c r="BC29" s="38"/>
+      <c r="BD29" s="34"/>
+      <c r="BE29" s="33"/>
+      <c r="BF29" s="34"/>
+      <c r="BG29" s="61"/>
+      <c r="BH29" s="62"/>
       <c r="BI29" s="48"/>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A30" s="57"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="5">
         <v>175000</v>
       </c>
@@ -18597,11 +18690,11 @@
         <v>1.75</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" ref="E30:E33" si="24">D30^2</f>
+        <f t="shared" ref="E30:E33" si="23">D30^2</f>
         <v>3.0625</v>
       </c>
       <c r="F30" s="11">
-        <f t="shared" ref="F30:F33" si="25">D30*LOG(D30,2)</f>
+        <f t="shared" ref="F30:F33" si="24">D30*LOG(D30,2)</f>
         <v>1.4128711136008072</v>
       </c>
       <c r="G30" s="17">
@@ -18624,7 +18717,7 @@
         <v>1.4014560000000001E-2</v>
       </c>
       <c r="M30" s="20">
-        <f t="shared" ref="M30:M33" si="26">L30/L29</f>
+        <f t="shared" ref="M30:M33" si="25">L30/L29</f>
         <v>1.7662680728357969</v>
       </c>
       <c r="N30" s="20">
@@ -18647,7 +18740,7 @@
         <v>4.6499799999999997E-3</v>
       </c>
       <c r="T30" s="20">
-        <f t="shared" ref="T30:T33" si="27">S30/S29</f>
+        <f t="shared" ref="T30:T33" si="26">S30/S29</f>
         <v>2.049099273778467</v>
       </c>
       <c r="U30" s="20">
@@ -18670,7 +18763,7 @@
         <v>7.9310400000000003E-3</v>
       </c>
       <c r="AA30" s="20">
-        <f t="shared" ref="AA30:AA33" si="28">Z30/Z29</f>
+        <f t="shared" ref="AA30:AA33" si="27">Z30/Z29</f>
         <v>1.8989589418942088</v>
       </c>
       <c r="AC30" s="48"/>
@@ -18709,7 +18802,7 @@
         <v>4.0372000000000003E-3</v>
       </c>
       <c r="AO30" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ30:AN30)</f>
         <v>4.6499799999999997E-3</v>
       </c>
       <c r="AP30" s="20">
@@ -18728,25 +18821,25 @@
         <v>7.8995000000000003E-3</v>
       </c>
       <c r="AU30" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.9310400000000003E-3</v>
       </c>
-      <c r="AX30" s="36"/>
-      <c r="AY30" s="36"/>
-      <c r="AZ30" s="37"/>
-      <c r="BA30" s="36"/>
-      <c r="BB30" s="37"/>
-      <c r="BC30" s="36"/>
-      <c r="BD30" s="37"/>
-      <c r="BE30" s="67"/>
-      <c r="BF30" s="37"/>
-      <c r="BG30" s="43"/>
-      <c r="BH30" s="44"/>
+      <c r="AX30" s="38"/>
+      <c r="AY30" s="38"/>
+      <c r="AZ30" s="34"/>
+      <c r="BA30" s="38"/>
+      <c r="BB30" s="34"/>
+      <c r="BC30" s="38"/>
+      <c r="BD30" s="34"/>
+      <c r="BE30" s="33"/>
+      <c r="BF30" s="34"/>
+      <c r="BG30" s="61"/>
+      <c r="BH30" s="62"/>
       <c r="BI30" s="48"/>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A31" s="57"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="5">
         <v>300000</v>
       </c>
@@ -18755,11 +18848,11 @@
         <v>1.7142857142857142</v>
       </c>
       <c r="E31" s="11">
+        <f t="shared" si="23"/>
+        <v>2.9387755102040813</v>
+      </c>
+      <c r="F31" s="11">
         <f t="shared" si="24"/>
-        <v>2.9387755102040813</v>
-      </c>
-      <c r="F31" s="11">
-        <f t="shared" si="25"/>
         <v>1.3330415634232318</v>
       </c>
       <c r="G31" s="17">
@@ -18782,7 +18875,7 @@
         <v>2.5084059999999998E-2</v>
       </c>
       <c r="M31" s="20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>1.7898571200237465</v>
       </c>
       <c r="N31" s="20">
@@ -18805,7 +18898,7 @@
         <v>6.4812399999999992E-3</v>
       </c>
       <c r="T31" s="20">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>1.3938210486926825</v>
       </c>
       <c r="U31" s="20">
@@ -18828,7 +18921,7 @@
         <v>1.3708639999999999E-2</v>
       </c>
       <c r="AA31" s="20">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>1.7284794932316567</v>
       </c>
       <c r="AC31" s="48"/>
@@ -18867,7 +18960,7 @@
         <v>6.5529000000000004E-3</v>
       </c>
       <c r="AO31" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ31:AN31)</f>
         <v>6.4812399999999992E-3</v>
       </c>
       <c r="AP31" s="20">
@@ -18886,25 +18979,25 @@
         <v>1.35464E-2</v>
       </c>
       <c r="AU31" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3708639999999999E-2</v>
       </c>
-      <c r="AX31" s="36"/>
-      <c r="AY31" s="36"/>
-      <c r="AZ31" s="37"/>
-      <c r="BA31" s="36"/>
-      <c r="BB31" s="37"/>
-      <c r="BC31" s="36"/>
-      <c r="BD31" s="37"/>
-      <c r="BE31" s="67"/>
-      <c r="BF31" s="37"/>
-      <c r="BG31" s="43"/>
-      <c r="BH31" s="44"/>
+      <c r="AX31" s="38"/>
+      <c r="AY31" s="38"/>
+      <c r="AZ31" s="34"/>
+      <c r="BA31" s="38"/>
+      <c r="BB31" s="34"/>
+      <c r="BC31" s="38"/>
+      <c r="BD31" s="34"/>
+      <c r="BE31" s="33"/>
+      <c r="BF31" s="34"/>
+      <c r="BG31" s="61"/>
+      <c r="BH31" s="62"/>
       <c r="BI31" s="48"/>
     </row>
     <row r="32" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="57"/>
-      <c r="B32" s="54"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="5">
         <v>425000</v>
       </c>
@@ -18913,11 +19006,11 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="E32" s="11">
+        <f t="shared" si="23"/>
+        <v>2.0069444444444446</v>
+      </c>
+      <c r="F32" s="11">
         <f t="shared" si="24"/>
-        <v>2.0069444444444446</v>
-      </c>
-      <c r="F32" s="11">
-        <f t="shared" si="25"/>
         <v>0.71187548241634313</v>
       </c>
       <c r="G32" s="17">
@@ -18940,7 +19033,7 @@
         <v>3.6373019999999999E-2</v>
       </c>
       <c r="M32" s="20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>1.4500451681266908</v>
       </c>
       <c r="N32" s="20">
@@ -18963,7 +19056,7 @@
         <v>1.0060419999999999E-2</v>
       </c>
       <c r="T32" s="20">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>1.5522369176268738</v>
       </c>
       <c r="U32" s="20">
@@ -18986,7 +19079,7 @@
         <v>1.9884720000000002E-2</v>
       </c>
       <c r="AA32" s="20">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>1.4505246326404371</v>
       </c>
       <c r="AC32" s="48"/>
@@ -19025,7 +19118,7 @@
         <v>9.6225000000000008E-3</v>
       </c>
       <c r="AO32" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ32:AN32)</f>
         <v>1.0060419999999999E-2</v>
       </c>
       <c r="AP32" s="20">
@@ -19044,25 +19137,25 @@
         <v>1.9841500000000001E-2</v>
       </c>
       <c r="AU32" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.9884720000000002E-2</v>
       </c>
-      <c r="AX32" s="38"/>
-      <c r="AY32" s="38"/>
-      <c r="AZ32" s="39"/>
-      <c r="BA32" s="38"/>
-      <c r="BB32" s="39"/>
-      <c r="BC32" s="38"/>
-      <c r="BD32" s="39"/>
-      <c r="BE32" s="68"/>
-      <c r="BF32" s="39"/>
-      <c r="BG32" s="45"/>
-      <c r="BH32" s="46"/>
+      <c r="AX32" s="39"/>
+      <c r="AY32" s="39"/>
+      <c r="AZ32" s="36"/>
+      <c r="BA32" s="39"/>
+      <c r="BB32" s="36"/>
+      <c r="BC32" s="39"/>
+      <c r="BD32" s="36"/>
+      <c r="BE32" s="35"/>
+      <c r="BF32" s="36"/>
+      <c r="BG32" s="63"/>
+      <c r="BH32" s="64"/>
       <c r="BI32" s="49"/>
     </row>
-    <row r="33" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="58"/>
-      <c r="B33" s="55"/>
+    <row r="33" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="55"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="6">
         <v>550000</v>
       </c>
@@ -19071,11 +19164,11 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="E33" s="11">
+        <f t="shared" si="23"/>
+        <v>1.6747404844290659</v>
+      </c>
+      <c r="F33" s="11">
         <f t="shared" si="24"/>
-        <v>1.6747404844290659</v>
-      </c>
-      <c r="F33" s="11">
-        <f t="shared" si="25"/>
         <v>0.48137135897135735</v>
       </c>
       <c r="G33" s="22">
@@ -19098,7 +19191,7 @@
         <v>4.7824020000000002E-2</v>
       </c>
       <c r="M33" s="20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>1.3148212603737606</v>
       </c>
       <c r="N33" s="25">
@@ -19121,7 +19214,7 @@
         <v>1.2501020000000002E-2</v>
       </c>
       <c r="T33" s="20">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>1.2425942455682768</v>
       </c>
       <c r="U33" s="25">
@@ -19144,7 +19237,7 @@
         <v>2.6853200000000001E-2</v>
       </c>
       <c r="AA33" s="20">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>1.350443958979558</v>
       </c>
       <c r="AC33" s="49"/>
@@ -19183,7 +19276,7 @@
         <v>1.26924E-2</v>
       </c>
       <c r="AO33" s="24">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ33:AN33)</f>
         <v>1.2501020000000002E-2</v>
       </c>
       <c r="AP33" s="25">
@@ -19202,41 +19295,41 @@
         <v>2.73493E-2</v>
       </c>
       <c r="AU33" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6853200000000001E-2</v>
       </c>
-      <c r="AX33" s="34" t="s">
+      <c r="AX33" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="AY33" s="62" t="s">
+      <c r="AY33" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="AZ33" s="35"/>
-      <c r="BA33" s="62" t="s">
+      <c r="AZ33" s="32"/>
+      <c r="BA33" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="BB33" s="35"/>
-      <c r="BC33" s="62" t="s">
+      <c r="BB33" s="32"/>
+      <c r="BC33" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="BD33" s="35"/>
-      <c r="BE33" s="66" t="s">
+      <c r="BD33" s="32"/>
+      <c r="BE33" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="BF33" s="35"/>
-      <c r="BG33" s="41" t="s">
+      <c r="BF33" s="32"/>
+      <c r="BG33" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="BH33" s="42"/>
+      <c r="BH33" s="60"/>
       <c r="BI33" s="48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A34" s="59" t="s">
+    <row r="34" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="A34" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="50" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="7">
@@ -19355,7 +19448,7 @@
         <v>1.1039000000000001E-3</v>
       </c>
       <c r="AO34" s="27">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ34:AN34)</f>
         <v>1.1025400000000002E-3</v>
       </c>
       <c r="AP34" s="13">
@@ -19374,25 +19467,25 @@
         <v>1.7941000000000001E-3</v>
       </c>
       <c r="AU34" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.7947400000000002E-3</v>
       </c>
-      <c r="AX34" s="36"/>
-      <c r="AY34" s="36"/>
-      <c r="AZ34" s="37"/>
-      <c r="BA34" s="36"/>
-      <c r="BB34" s="37"/>
-      <c r="BC34" s="36"/>
-      <c r="BD34" s="37"/>
-      <c r="BE34" s="67"/>
-      <c r="BF34" s="37"/>
-      <c r="BG34" s="43"/>
-      <c r="BH34" s="44"/>
+      <c r="AX34" s="38"/>
+      <c r="AY34" s="38"/>
+      <c r="AZ34" s="34"/>
+      <c r="BA34" s="38"/>
+      <c r="BB34" s="34"/>
+      <c r="BC34" s="38"/>
+      <c r="BD34" s="34"/>
+      <c r="BE34" s="33"/>
+      <c r="BF34" s="34"/>
+      <c r="BG34" s="61"/>
+      <c r="BH34" s="62"/>
       <c r="BI34" s="48"/>
     </row>
-    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A35" s="57"/>
-      <c r="B35" s="54"/>
+    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="A35" s="54"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="5">
         <v>100000</v>
       </c>
@@ -19513,7 +19606,7 @@
         <v>2.1654000000000001E-3</v>
       </c>
       <c r="AO35" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ35:AN35)</f>
         <v>2.2882999999999996E-3</v>
       </c>
       <c r="AP35" s="20">
@@ -19532,25 +19625,25 @@
         <v>3.4102E-3</v>
       </c>
       <c r="AU35" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2638199999999997E-3</v>
       </c>
-      <c r="AX35" s="36"/>
-      <c r="AY35" s="36"/>
-      <c r="AZ35" s="37"/>
-      <c r="BA35" s="36"/>
-      <c r="BB35" s="37"/>
-      <c r="BC35" s="36"/>
-      <c r="BD35" s="37"/>
-      <c r="BE35" s="67"/>
-      <c r="BF35" s="37"/>
-      <c r="BG35" s="43"/>
-      <c r="BH35" s="44"/>
+      <c r="AX35" s="38"/>
+      <c r="AY35" s="38"/>
+      <c r="AZ35" s="34"/>
+      <c r="BA35" s="38"/>
+      <c r="BB35" s="34"/>
+      <c r="BC35" s="38"/>
+      <c r="BD35" s="34"/>
+      <c r="BE35" s="33"/>
+      <c r="BF35" s="34"/>
+      <c r="BG35" s="61"/>
+      <c r="BH35" s="62"/>
       <c r="BI35" s="48"/>
     </row>
-    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A36" s="57"/>
-      <c r="B36" s="54"/>
+    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="A36" s="54"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="5">
         <v>175000</v>
       </c>
@@ -19559,11 +19652,11 @@
         <v>1.75</v>
       </c>
       <c r="E36" s="11">
-        <f t="shared" ref="E36:E39" si="29">D36^2</f>
+        <f t="shared" ref="E36:E39" si="28">D36^2</f>
         <v>3.0625</v>
       </c>
       <c r="F36" s="11">
-        <f t="shared" ref="F36:F39" si="30">D36*LOG(D36,2)</f>
+        <f t="shared" ref="F36:F39" si="29">D36*LOG(D36,2)</f>
         <v>1.4128711136008072</v>
       </c>
       <c r="G36" s="17">
@@ -19586,7 +19679,7 @@
         <v>2.9459000000000003E-2</v>
       </c>
       <c r="M36" s="20">
-        <f t="shared" ref="M36:M39" si="31">L36/L35</f>
+        <f t="shared" ref="M36:M39" si="30">L36/L35</f>
         <v>1.814312988852621</v>
       </c>
       <c r="N36" s="20">
@@ -19609,7 +19702,7 @@
         <v>4.0748200000000007E-3</v>
       </c>
       <c r="T36" s="20">
-        <f t="shared" ref="T36:T39" si="32">S36/S35</f>
+        <f t="shared" ref="T36:T39" si="31">S36/S35</f>
         <v>1.7807193112791162</v>
       </c>
       <c r="U36" s="20">
@@ -19632,7 +19725,7 @@
         <v>6.2572799999999996E-3</v>
       </c>
       <c r="AA36" s="20">
-        <f t="shared" ref="AA36:AA39" si="33">Z36/Z35</f>
+        <f t="shared" ref="AA36:AA39" si="32">Z36/Z35</f>
         <v>1.9171645495155982</v>
       </c>
       <c r="AC36" s="48"/>
@@ -19671,7 +19764,7 @@
         <v>4.1980999999999997E-3</v>
       </c>
       <c r="AO36" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ36:AN36)</f>
         <v>4.0748200000000007E-3</v>
       </c>
       <c r="AP36" s="20">
@@ -19690,25 +19783,25 @@
         <v>6.6128000000000003E-3</v>
       </c>
       <c r="AU36" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.2572799999999996E-3</v>
       </c>
-      <c r="AX36" s="36"/>
-      <c r="AY36" s="36"/>
-      <c r="AZ36" s="37"/>
-      <c r="BA36" s="36"/>
-      <c r="BB36" s="37"/>
-      <c r="BC36" s="36"/>
-      <c r="BD36" s="37"/>
-      <c r="BE36" s="67"/>
-      <c r="BF36" s="37"/>
-      <c r="BG36" s="43"/>
-      <c r="BH36" s="44"/>
+      <c r="AX36" s="38"/>
+      <c r="AY36" s="38"/>
+      <c r="AZ36" s="34"/>
+      <c r="BA36" s="38"/>
+      <c r="BB36" s="34"/>
+      <c r="BC36" s="38"/>
+      <c r="BD36" s="34"/>
+      <c r="BE36" s="33"/>
+      <c r="BF36" s="34"/>
+      <c r="BG36" s="61"/>
+      <c r="BH36" s="62"/>
       <c r="BI36" s="48"/>
     </row>
-    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="A37" s="57"/>
-      <c r="B37" s="54"/>
+    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="A37" s="54"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="5">
         <v>300000</v>
       </c>
@@ -19717,11 +19810,11 @@
         <v>1.7142857142857142</v>
       </c>
       <c r="E37" s="11">
+        <f t="shared" si="28"/>
+        <v>2.9387755102040813</v>
+      </c>
+      <c r="F37" s="11">
         <f t="shared" si="29"/>
-        <v>2.9387755102040813</v>
-      </c>
-      <c r="F37" s="11">
-        <f t="shared" si="30"/>
         <v>1.3330415634232318</v>
       </c>
       <c r="G37" s="17">
@@ -19744,7 +19837,7 @@
         <v>5.6187880000000003E-2</v>
       </c>
       <c r="M37" s="20">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>1.9073247564411555</v>
       </c>
       <c r="N37" s="20">
@@ -19767,7 +19860,7 @@
         <v>7.2292599999999995E-3</v>
       </c>
       <c r="T37" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>1.7741299002164508</v>
       </c>
       <c r="U37" s="20">
@@ -19790,7 +19883,7 @@
         <v>1.0778959999999999E-2</v>
       </c>
       <c r="AA37" s="20">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>1.7226270839725886</v>
       </c>
       <c r="AC37" s="48"/>
@@ -19829,7 +19922,7 @@
         <v>7.2224000000000003E-3</v>
       </c>
       <c r="AO37" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ37:AN37)</f>
         <v>7.2292599999999995E-3</v>
       </c>
       <c r="AP37" s="20">
@@ -19848,25 +19941,25 @@
         <v>1.09687E-2</v>
       </c>
       <c r="AU37" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.0778959999999999E-2</v>
       </c>
-      <c r="AX37" s="36"/>
-      <c r="AY37" s="36"/>
-      <c r="AZ37" s="37"/>
-      <c r="BA37" s="36"/>
-      <c r="BB37" s="37"/>
-      <c r="BC37" s="36"/>
-      <c r="BD37" s="37"/>
-      <c r="BE37" s="67"/>
-      <c r="BF37" s="37"/>
-      <c r="BG37" s="43"/>
-      <c r="BH37" s="44"/>
+      <c r="AX37" s="38"/>
+      <c r="AY37" s="38"/>
+      <c r="AZ37" s="34"/>
+      <c r="BA37" s="38"/>
+      <c r="BB37" s="34"/>
+      <c r="BC37" s="38"/>
+      <c r="BD37" s="34"/>
+      <c r="BE37" s="33"/>
+      <c r="BF37" s="34"/>
+      <c r="BG37" s="61"/>
+      <c r="BH37" s="62"/>
       <c r="BI37" s="48"/>
     </row>
-    <row r="38" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="57"/>
-      <c r="B38" s="54"/>
+    <row r="38" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="54"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="5">
         <v>425000</v>
       </c>
@@ -19875,11 +19968,11 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="E38" s="11">
+        <f t="shared" si="28"/>
+        <v>2.0069444444444446</v>
+      </c>
+      <c r="F38" s="11">
         <f t="shared" si="29"/>
-        <v>2.0069444444444446</v>
-      </c>
-      <c r="F38" s="11">
-        <f t="shared" si="30"/>
         <v>0.71187548241634313</v>
       </c>
       <c r="G38" s="17">
@@ -19902,7 +19995,7 @@
         <v>8.0770339999999996E-2</v>
       </c>
       <c r="M38" s="20">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>1.4375046718260236</v>
       </c>
       <c r="N38" s="20">
@@ -19925,7 +20018,7 @@
         <v>1.0179200000000001E-2</v>
       </c>
       <c r="T38" s="20">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>1.4080555962850971</v>
       </c>
       <c r="U38" s="20">
@@ -19948,7 +20041,7 @@
         <v>1.5200720000000001E-2</v>
       </c>
       <c r="AA38" s="20">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>1.4102213942718038</v>
       </c>
       <c r="AC38" s="48"/>
@@ -19987,7 +20080,7 @@
         <v>1.06573E-2</v>
       </c>
       <c r="AO38" s="19">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ38:AN38)</f>
         <v>1.0179200000000001E-2</v>
       </c>
       <c r="AP38" s="20">
@@ -20006,25 +20099,25 @@
         <v>1.5428799999999999E-2</v>
       </c>
       <c r="AU38" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.5200720000000001E-2</v>
       </c>
-      <c r="AX38" s="38"/>
-      <c r="AY38" s="38"/>
-      <c r="AZ38" s="39"/>
-      <c r="BA38" s="38"/>
-      <c r="BB38" s="39"/>
-      <c r="BC38" s="38"/>
-      <c r="BD38" s="39"/>
-      <c r="BE38" s="68"/>
-      <c r="BF38" s="39"/>
-      <c r="BG38" s="45"/>
-      <c r="BH38" s="46"/>
+      <c r="AX38" s="39"/>
+      <c r="AY38" s="39"/>
+      <c r="AZ38" s="36"/>
+      <c r="BA38" s="39"/>
+      <c r="BB38" s="36"/>
+      <c r="BC38" s="39"/>
+      <c r="BD38" s="36"/>
+      <c r="BE38" s="35"/>
+      <c r="BF38" s="36"/>
+      <c r="BG38" s="63"/>
+      <c r="BH38" s="64"/>
       <c r="BI38" s="49"/>
     </row>
-    <row r="39" spans="1:61" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="58"/>
-      <c r="B39" s="55"/>
+    <row r="39" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="55"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="6">
         <v>550000</v>
       </c>
@@ -20033,11 +20126,11 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="E39" s="12">
+        <f t="shared" si="28"/>
+        <v>1.6747404844290659</v>
+      </c>
+      <c r="F39" s="12">
         <f t="shared" si="29"/>
-        <v>1.6747404844290659</v>
-      </c>
-      <c r="F39" s="12">
-        <f t="shared" si="30"/>
         <v>0.48137135897135735</v>
       </c>
       <c r="G39" s="22">
@@ -20060,7 +20153,7 @@
         <v>0.10898352</v>
       </c>
       <c r="M39" s="23">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>1.3493012410248615</v>
       </c>
       <c r="N39" s="25">
@@ -20083,7 +20176,7 @@
         <v>1.385656E-2</v>
       </c>
       <c r="T39" s="23">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>1.3612621817038666</v>
       </c>
       <c r="U39" s="25">
@@ -20106,7 +20199,7 @@
         <v>2.0551239999999998E-2</v>
       </c>
       <c r="AA39" s="23">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>1.3519912214684566</v>
       </c>
       <c r="AC39" s="49"/>
@@ -20145,7 +20238,7 @@
         <v>1.36262E-2</v>
       </c>
       <c r="AO39" s="24">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(AJ39:AN39)</f>
         <v>1.385656E-2</v>
       </c>
       <c r="AP39" s="25">
@@ -20164,1007 +20257,1013 @@
         <v>2.0744599999999998E-2</v>
       </c>
       <c r="AU39" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.0551239999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="AI45" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK45" t="s">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BL40" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="BM40" s="73"/>
+      <c r="BN40" s="73"/>
+      <c r="BO40" s="73"/>
+      <c r="BP40" s="73"/>
+      <c r="BQ40" s="74"/>
+    </row>
+    <row r="41" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL41" s="75"/>
+      <c r="BM41" s="76"/>
+      <c r="BN41" s="76"/>
+      <c r="BO41" s="76"/>
+      <c r="BP41" s="76"/>
+      <c r="BQ41" s="77"/>
+    </row>
+    <row r="42" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL42" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="BM42" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="AM45" t="s">
+      <c r="BN42" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="AO45" t="s">
+      <c r="BO42" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="AQ45" t="s">
+      <c r="BP42" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AS45" t="s">
+      <c r="BQ42" s="79" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="AI46">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BL43" s="69">
         <f>$AI$34/AI4</f>
         <v>1.9753604834412252E-3</v>
       </c>
-      <c r="AK46">
+      <c r="BM43" s="70">
         <f>AI28/AI4</f>
         <v>9.6843513525073229E-4</v>
       </c>
-      <c r="AM46">
+      <c r="BN43" s="71">
         <f>AI22/AI4</f>
         <v>7.0904596849602538E-3</v>
       </c>
-      <c r="AO46">
+      <c r="BO43" s="82">
         <f>AI16/AI4</f>
         <v>0.14564946155704886</v>
       </c>
-      <c r="AQ46">
+      <c r="BP43" s="83">
         <f>AI10/AI4</f>
         <v>0.2259003724994392</v>
       </c>
-      <c r="AS46" s="30">
+      <c r="BQ43" s="84">
         <f>AI4/AI10</f>
         <v>4.4267301949777993</v>
       </c>
     </row>
-    <row r="47" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="AI47">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BL44" s="69">
         <f>$AI$35/AI5</f>
         <v>9.9029751783332961E-4</v>
       </c>
-      <c r="AK47">
-        <f t="shared" ref="AK47:AK50" si="34">AI29/AI5</f>
+      <c r="BM44" s="70">
+        <f>AI29/AI5</f>
         <v>4.8393022560199697E-4</v>
       </c>
-      <c r="AM47">
-        <f t="shared" ref="AM47:AM50" si="35">AI23/AI5</f>
+      <c r="BN44" s="71">
+        <f>AI23/AI5</f>
         <v>3.0252982317538566E-3</v>
       </c>
-      <c r="AO47">
-        <f t="shared" ref="AO47:AO50" si="36">AI17/AI5</f>
+      <c r="BO44" s="82">
+        <f>AI17/AI5</f>
         <v>0.13502435798277596</v>
       </c>
-      <c r="AQ47">
-        <f t="shared" ref="AQ47:AQ51" si="37">AI11/AI5</f>
+      <c r="BP44" s="83">
+        <f>AI11/AI5</f>
         <v>0.21136013787000474</v>
       </c>
-      <c r="AS47" s="30">
-        <f t="shared" ref="AS47:AS51" si="38">AI5/AI11</f>
+      <c r="BQ44" s="84">
+        <f>AI5/AI11</f>
         <v>4.7312611075937205</v>
       </c>
     </row>
-    <row r="48" spans="1:61" x14ac:dyDescent="0.35">
-      <c r="AI48">
+    <row r="45" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BL45" s="69">
         <f>$AI$36/AI6</f>
         <v>5.9580279467660554E-4</v>
       </c>
-      <c r="AK48">
-        <f t="shared" si="34"/>
+      <c r="BM45" s="70">
+        <f>AI30/AI6</f>
         <v>2.8344186884018355E-4</v>
       </c>
-      <c r="AM48">
-        <f t="shared" si="35"/>
+      <c r="BN45" s="71">
+        <f>AI24/AI6</f>
         <v>1.7024273562037512E-3</v>
       </c>
-      <c r="AO48">
-        <f t="shared" si="36"/>
+      <c r="BO45" s="82">
+        <f>AI18/AI6</f>
         <v>0.1389270474723702</v>
       </c>
-      <c r="AQ48">
-        <f t="shared" si="37"/>
+      <c r="BP45" s="83">
+        <f>AI12/AI6</f>
         <v>0.22063037682291717</v>
       </c>
-      <c r="AS48" s="30">
-        <f t="shared" si="38"/>
+      <c r="BQ45" s="84">
+        <f>AI6/AI12</f>
         <v>4.5324674435135561</v>
       </c>
     </row>
-    <row r="49" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI49">
+    <row r="46" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BL46" s="69">
         <f>$AI$37/AI7</f>
         <v>3.7249745694266964E-4</v>
       </c>
-      <c r="AK49">
-        <f t="shared" si="34"/>
+      <c r="BM46" s="70">
+        <f>AI31/AI7</f>
         <v>1.6629473402088389E-4</v>
       </c>
-      <c r="AM49">
-        <f t="shared" si="35"/>
+      <c r="BN46" s="71">
+        <f>AI25/AI7</f>
         <v>9.7028953129401035E-4</v>
       </c>
-      <c r="AO49">
-        <f t="shared" si="36"/>
+      <c r="BO46" s="82">
+        <f>AI19/AI7</f>
         <v>0.13352583840777735</v>
       </c>
-      <c r="AQ49">
-        <f t="shared" si="37"/>
+      <c r="BP46" s="83">
+        <f>AI13/AI7</f>
         <v>0.20901427367520201</v>
       </c>
-      <c r="AS49" s="30">
-        <f t="shared" si="38"/>
+      <c r="BQ46" s="84">
+        <f>AI7/AI13</f>
         <v>4.7843622467332123</v>
       </c>
     </row>
-    <row r="50" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI50">
+    <row r="47" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BL47" s="69">
         <f>$AI$38/AI8</f>
         <v>2.6251916182252496E-4</v>
       </c>
-      <c r="AK50">
-        <f t="shared" si="34"/>
+      <c r="BM47" s="70">
+        <f>AI32/AI8</f>
         <v>1.1821932064856899E-4</v>
       </c>
-      <c r="AM50">
-        <f t="shared" si="35"/>
+      <c r="BN47" s="71">
+        <f>AI26/AI8</f>
         <v>6.6905734817787924E-4</v>
       </c>
-      <c r="AO50">
-        <f t="shared" si="36"/>
+      <c r="BO47" s="82">
+        <f>AI20/AI8</f>
         <v>0.13105270602190622</v>
       </c>
-      <c r="AQ50">
-        <f t="shared" si="37"/>
+      <c r="BP47" s="83">
+        <f>AI14/AI8</f>
         <v>0.21679792479799201</v>
       </c>
-      <c r="AS50" s="30">
-        <f t="shared" si="38"/>
+      <c r="BQ47" s="84">
+        <f>AI8/AI14</f>
         <v>4.6125902770138607</v>
       </c>
     </row>
-    <row r="51" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI51">
+    <row r="48" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL48" s="69">
         <f>$AI$39/AI9</f>
         <v>2.2031309066109241E-4</v>
       </c>
-      <c r="AK51">
+      <c r="BM48" s="70">
         <f>AI33/AI9</f>
         <v>9.6677531190384535E-5</v>
       </c>
-      <c r="AM51">
+      <c r="BN48" s="71">
         <f>AI27/AI9</f>
         <v>5.3742128450283769E-4</v>
       </c>
-      <c r="AO51">
+      <c r="BO48" s="82">
         <f>AI21/AI9</f>
         <v>0.13398558386003684</v>
       </c>
-      <c r="AQ51">
-        <f t="shared" si="37"/>
+      <c r="BP48" s="83">
+        <f>AI15/AI9</f>
         <v>0.2218091667444945</v>
       </c>
-      <c r="AS51" s="30">
-        <f t="shared" si="38"/>
+      <c r="BQ48" s="84">
+        <f>AI9/AI15</f>
         <v>4.5083799496524684</v>
       </c>
     </row>
-    <row r="52" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI52" t="s">
+    <row r="49" spans="48:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL49" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM49" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="AK52" t="s">
+      <c r="BN49" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="AM52" t="s">
+      <c r="BO49" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="AO52" t="s">
+      <c r="BP49" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ49" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="AQ52" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS52" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="53" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI53">
+    <row r="50" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="BL50" s="69">
         <f>$AI$34/AI10</f>
         <v>8.7443878980152153E-3</v>
       </c>
-      <c r="AK53">
+      <c r="BM50" s="70">
         <f>AI28/AI10</f>
         <v>4.2870010550918256E-3</v>
       </c>
-      <c r="AM53">
+      <c r="BN50" s="71">
         <f>AI22/AI10</f>
         <v>3.1387551983686326E-2</v>
       </c>
-      <c r="AO53">
+      <c r="BO50" s="82">
         <f>AI16/AI10</f>
         <v>0.64475086935684645</v>
       </c>
-      <c r="AQ53">
+      <c r="BP50" s="83">
         <f>AI10/AI16</f>
         <v>1.5509866640389685</v>
       </c>
-      <c r="AS53">
+      <c r="BQ50" s="82">
         <f>AI4/AI16</f>
         <v>6.8657994977091894</v>
       </c>
     </row>
-    <row r="54" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI54">
+    <row r="51" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="BL51" s="69">
         <f>$AI$35/AI11</f>
         <v>4.6853561310714314E-3</v>
       </c>
-      <c r="AK54">
-        <f t="shared" ref="AK54:AK58" si="39">AI29/AI11</f>
+      <c r="BM51" s="70">
+        <f>AI29/AI11</f>
         <v>2.2896002551797833E-3</v>
       </c>
-      <c r="AM54">
-        <f t="shared" ref="AM54:AM58" si="40">AI23/AI11</f>
+      <c r="BN51" s="71">
+        <f>AI23/AI11</f>
         <v>1.4313475862769076E-2</v>
       </c>
-      <c r="AO54">
-        <f t="shared" ref="AO54:AO58" si="41">AI17/AI11</f>
+      <c r="BO51" s="82">
+        <f>AI17/AI11</f>
         <v>0.63883549350171953</v>
       </c>
-      <c r="AQ54">
-        <f t="shared" ref="AQ54:AQ58" si="42">AI11/AI17</f>
+      <c r="BP51" s="83">
+        <f>AI11/AI17</f>
         <v>1.5653482158898053</v>
       </c>
-      <c r="AS54">
-        <f t="shared" ref="AS54:AS57" si="43">AI5/AI17</f>
+      <c r="BQ51" s="82">
+        <f>AI5/AI17</f>
         <v>7.406071133680654</v>
       </c>
     </row>
-    <row r="55" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI55">
+    <row r="52" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="BL52" s="69">
         <f>$AI$36/AI12</f>
         <v>2.7004567696261063E-3</v>
       </c>
-      <c r="AK55">
-        <f t="shared" si="39"/>
+      <c r="BM52" s="70">
+        <f>AI30/AI12</f>
         <v>1.2846910426467717E-3</v>
       </c>
-      <c r="AM55">
-        <f t="shared" si="40"/>
+      <c r="BN52" s="71">
+        <f>AI24/AI12</f>
         <v>7.7161965669403582E-3</v>
       </c>
-      <c r="AO55">
-        <f t="shared" si="41"/>
+      <c r="BO52" s="82">
+        <f>AI18/AI12</f>
         <v>0.62968231969198019</v>
       </c>
-      <c r="AQ55">
-        <f t="shared" si="42"/>
+      <c r="BP52" s="83">
+        <f>AI12/AI18</f>
         <v>1.5881023950127218</v>
       </c>
-      <c r="AS55">
-        <f t="shared" si="43"/>
+      <c r="BQ52" s="82">
+        <f>AI6/AI18</f>
         <v>7.1980224023610671</v>
       </c>
-      <c r="AV55" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW55" s="40"/>
-      <c r="AX55" s="40"/>
-      <c r="AY55" s="40"/>
     </row>
-    <row r="56" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI56">
+    <row r="53" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="BL53" s="69">
         <f>$AI$37/AI13</f>
         <v>1.7821627700006391E-3</v>
       </c>
-      <c r="AK56">
-        <f t="shared" si="39"/>
+      <c r="BM53" s="70">
+        <f>AI31/AI13</f>
         <v>7.9561424728005802E-4</v>
       </c>
-      <c r="AM56">
-        <f t="shared" si="40"/>
+      <c r="BN53" s="71">
+        <f>AI25/AI13</f>
         <v>4.6422166019235269E-3</v>
       </c>
-      <c r="AO56">
-        <f t="shared" si="41"/>
+      <c r="BO53" s="82">
+        <f>AI19/AI13</f>
         <v>0.63883598024156951</v>
       </c>
-      <c r="AQ56">
-        <f t="shared" si="42"/>
+      <c r="BP53" s="83">
+        <f>AI13/AI19</f>
         <v>1.5653470232247406</v>
       </c>
-      <c r="AS56">
-        <f t="shared" si="43"/>
+      <c r="BQ53" s="82">
+        <f>AI7/AI19</f>
         <v>7.4891872009526663</v>
       </c>
-      <c r="AV56" s="40"/>
-      <c r="AW56" s="40"/>
-      <c r="AX56" s="40"/>
-      <c r="AY56" s="40"/>
     </row>
-    <row r="57" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI57">
+    <row r="54" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="BL54" s="69">
         <f>$AI$38/AI14</f>
         <v>1.2108933333524069E-3</v>
       </c>
-      <c r="AK57">
-        <f t="shared" si="39"/>
+      <c r="BM54" s="70">
+        <f>AI32/AI14</f>
         <v>5.4529728897877324E-4</v>
       </c>
-      <c r="AM57">
-        <f t="shared" si="40"/>
+      <c r="BN54" s="71">
+        <f>AI26/AI14</f>
         <v>3.0860874189699628E-3</v>
       </c>
-      <c r="AO57">
-        <f t="shared" si="41"/>
+      <c r="BO54" s="82">
+        <f>AI20/AI14</f>
         <v>0.60449243757300042</v>
       </c>
-      <c r="AQ57">
-        <f t="shared" si="42"/>
+      <c r="BP54" s="83">
+        <f>AI14/AI20</f>
         <v>1.6542804141850607</v>
       </c>
-      <c r="AS57">
-        <f t="shared" si="43"/>
+      <c r="BQ54" s="82">
+        <f>AI8/AI20</f>
         <v>7.6305177539244724</v>
       </c>
-      <c r="AV57" s="40"/>
-      <c r="AW57" s="40"/>
-      <c r="AX57" s="40"/>
-      <c r="AY57" s="40"/>
     </row>
-    <row r="58" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI58">
+    <row r="55" spans="48:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AV55" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW55" s="58"/>
+      <c r="AX55" s="58"/>
+      <c r="AY55" s="58"/>
+      <c r="BL55" s="69">
         <f>$AI$39/AI15</f>
         <v>9.9325512058243549E-4</v>
       </c>
-      <c r="AK58">
-        <f t="shared" si="39"/>
+      <c r="BM55" s="70">
+        <f>AI33/AI15</f>
         <v>4.3585904320063076E-4</v>
       </c>
-      <c r="AM58">
-        <f t="shared" si="40"/>
+      <c r="BN55" s="71">
+        <f>AI27/AI15</f>
         <v>2.4228993435690682E-3</v>
       </c>
-      <c r="AO58">
-        <f t="shared" si="41"/>
+      <c r="BO55" s="82">
+        <f>AI21/AI15</f>
         <v>0.60405791981706947</v>
       </c>
-      <c r="AQ58">
-        <f t="shared" si="42"/>
+      <c r="BP55" s="83">
+        <f>AI15/AI21</f>
         <v>1.6554703898308893</v>
       </c>
-      <c r="AS58">
+      <c r="BQ55" s="82">
         <f>AI9/AI21</f>
         <v>7.4634895127569365</v>
       </c>
-      <c r="AV58" s="40"/>
-      <c r="AW58" s="40"/>
-      <c r="AX58" s="40"/>
-      <c r="AY58" s="40"/>
     </row>
-    <row r="59" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI59" t="s">
+    <row r="56" spans="48:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AV56" s="58"/>
+      <c r="AW56" s="58"/>
+      <c r="AX56" s="58"/>
+      <c r="AY56" s="58"/>
+      <c r="BL56" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="BM56" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="BN56" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="AK59" t="s">
+      <c r="BO56" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="AM59" t="s">
+      <c r="BP56" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="AO59" t="s">
+      <c r="BQ56" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="AQ59" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS59" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV59" s="40"/>
-      <c r="AW59" s="40"/>
-      <c r="AX59" s="40"/>
-      <c r="AY59" s="40"/>
     </row>
-    <row r="60" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI60">
+    <row r="57" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="AV57" s="58"/>
+      <c r="AW57" s="58"/>
+      <c r="AX57" s="58"/>
+      <c r="AY57" s="58"/>
+      <c r="BL57" s="69">
         <f>$AI$34/AI16</f>
         <v>1.3562429015005345E-2</v>
       </c>
-      <c r="AK60">
+      <c r="BM57" s="70">
         <f>AI28/AI16</f>
         <v>6.6490814651684084E-3</v>
       </c>
-      <c r="AM60">
+      <c r="BN57" s="71">
         <f>AI22/AI16</f>
         <v>4.8681674543527363E-2</v>
       </c>
-      <c r="AO60" s="33">
+      <c r="BO57" s="85">
         <f>AI16/AI22</f>
         <v>20.541610562427916</v>
       </c>
-      <c r="AQ60">
+      <c r="BP57" s="83">
         <f>AI10/AI22</f>
         <v>31.859764040207715</v>
       </c>
-      <c r="AS60">
+      <c r="BQ57" s="86">
         <f>AI4/AI22</f>
         <v>141.03457948165538</v>
       </c>
-      <c r="AV60" s="40"/>
-      <c r="AW60" s="40"/>
-      <c r="AX60" s="40"/>
-      <c r="AY60" s="40"/>
     </row>
-    <row r="61" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI61">
+    <row r="58" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="AV58" s="58"/>
+      <c r="AW58" s="58"/>
+      <c r="AX58" s="58"/>
+      <c r="AY58" s="58"/>
+      <c r="BL58" s="69">
         <f>$AI$35/AI17</f>
         <v>7.3342138605810257E-3</v>
       </c>
-      <c r="AK61">
-        <f t="shared" ref="AK61:AK65" si="44">AI29/AI17</f>
+      <c r="BM58" s="70">
+        <f>AI29/AI17</f>
         <v>3.5840216745465165E-3</v>
       </c>
-      <c r="AM61">
-        <f t="shared" ref="AM61:AM65" si="45">AI23/AI17</f>
+      <c r="BN58" s="71">
+        <f>AI23/AI17</f>
         <v>2.2405573904967363E-2</v>
       </c>
-      <c r="AO61">
-        <f t="shared" ref="AO61:AO65" si="46">AI17/AI23</f>
+      <c r="BO58" s="82">
+        <f>AI17/AI23</f>
         <v>44.631751199120046</v>
       </c>
-      <c r="AQ61">
-        <f t="shared" ref="AQ61:AQ65" si="47">AI11/AI23</f>
+      <c r="BP58" s="83">
+        <f>AI11/AI23</f>
         <v>69.86423211158025</v>
       </c>
-      <c r="AS61">
-        <f t="shared" ref="AS61:AS65" si="48">AI5/AI23</f>
+      <c r="BQ58" s="82">
+        <f>AI5/AI23</f>
         <v>330.54592420141995</v>
       </c>
-      <c r="AV61" s="40"/>
-      <c r="AW61" s="40"/>
-      <c r="AX61" s="40"/>
-      <c r="AY61" s="40"/>
     </row>
-    <row r="62" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI62">
+    <row r="59" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="AV59" s="58"/>
+      <c r="AW59" s="58"/>
+      <c r="AX59" s="58"/>
+      <c r="AY59" s="58"/>
+      <c r="BL59" s="69">
         <f>$AI$36/AI18</f>
         <v>4.2886018634715369E-3</v>
       </c>
-      <c r="AK62">
-        <f t="shared" si="44"/>
+      <c r="BM59" s="70">
+        <f>AI30/AI18</f>
         <v>2.0402209216787287E-3</v>
       </c>
-      <c r="AM62">
-        <f t="shared" si="45"/>
+      <c r="BN59" s="71">
+        <f>AI24/AI18</f>
         <v>1.2254110248346925E-2</v>
       </c>
-      <c r="AO62" s="32">
-        <f t="shared" si="46"/>
+      <c r="BO59" s="86">
+        <f>AI18/AI24</f>
         <v>81.605272005358344</v>
       </c>
-      <c r="AQ62">
-        <f t="shared" si="47"/>
+      <c r="BP59" s="83">
+        <f>AI12/AI24</f>
         <v>129.59752791737418</v>
       </c>
-      <c r="AS62">
-        <f t="shared" si="48"/>
+      <c r="BQ59" s="82">
+        <f>AI6/AI24</f>
         <v>587.39657604533772</v>
       </c>
-      <c r="AV62" s="40"/>
-      <c r="AW62" s="40"/>
-      <c r="AX62" s="40"/>
-      <c r="AY62" s="40"/>
     </row>
-    <row r="63" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI63">
+    <row r="60" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="AV60" s="58"/>
+      <c r="AW60" s="58"/>
+      <c r="AX60" s="58"/>
+      <c r="AY60" s="58"/>
+      <c r="BL60" s="69">
         <f>$AI$37/AI19</f>
         <v>2.7897031869224581E-3</v>
       </c>
-      <c r="AK63">
-        <f t="shared" si="44"/>
+      <c r="BM60" s="70">
+        <f>AI31/AI19</f>
         <v>1.2454123936150314E-3</v>
       </c>
-      <c r="AM63">
-        <f t="shared" si="45"/>
+      <c r="BN60" s="71">
+        <f>AI25/AI19</f>
         <v>7.266679938985463E-3</v>
       </c>
-      <c r="AO63">
-        <f t="shared" si="46"/>
+      <c r="BO60" s="82">
+        <f>AI19/AI25</f>
         <v>137.61442755102476</v>
       </c>
-      <c r="AQ63">
-        <f t="shared" si="47"/>
+      <c r="BP60" s="83">
+        <f>AI13/AI25</f>
         <v>215.41433451977332</v>
       </c>
-      <c r="AS63">
-        <f t="shared" si="48"/>
+      <c r="BQ60" s="82">
+        <f>AI7/AI25</f>
         <v>1030.6202094815626</v>
       </c>
-      <c r="AV63" s="40"/>
-      <c r="AW63" s="40"/>
-      <c r="AX63" s="40"/>
-      <c r="AY63" s="40"/>
     </row>
-    <row r="64" spans="35:51" x14ac:dyDescent="0.35">
-      <c r="AI64">
+    <row r="61" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="AV61" s="58"/>
+      <c r="AW61" s="58"/>
+      <c r="AX61" s="58"/>
+      <c r="AY61" s="58"/>
+      <c r="BL61" s="69">
         <f>$AI$38/AI20</f>
         <v>2.0031571250321485E-3</v>
       </c>
-      <c r="AK64">
-        <f t="shared" si="44"/>
+      <c r="BM61" s="70">
+        <f>AI32/AI20</f>
         <v>9.0207462506579567E-4</v>
       </c>
-      <c r="AM64">
-        <f t="shared" si="45"/>
+      <c r="BN61" s="71">
+        <f>AI26/AI20</f>
         <v>5.1052539736649348E-3</v>
       </c>
-      <c r="AO64">
-        <f t="shared" si="46"/>
+      <c r="BO61" s="82">
+        <f>AI20/AI26</f>
         <v>195.87664103655257</v>
       </c>
-      <c r="AQ64">
-        <f t="shared" si="47"/>
+      <c r="BP61" s="83">
+        <f>AI14/AI26</f>
         <v>324.03489086312663</v>
       </c>
-      <c r="AS64">
-        <f t="shared" si="48"/>
+      <c r="BQ61" s="82">
+        <f>AI8/AI26</f>
         <v>1494.6401870085053</v>
       </c>
     </row>
-    <row r="65" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI65">
+    <row r="62" spans="48:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AV62" s="58"/>
+      <c r="AW62" s="58"/>
+      <c r="AX62" s="58"/>
+      <c r="AY62" s="58"/>
+      <c r="BL62" s="69">
         <f>$AI$39/AI21</f>
         <v>1.6443044416721315E-3</v>
       </c>
-      <c r="AK65">
-        <f t="shared" si="44"/>
+      <c r="BM62" s="70">
+        <f>AI33/AI21</f>
         <v>7.2155174015866663E-4</v>
       </c>
-      <c r="AM65">
-        <f t="shared" si="45"/>
+      <c r="BN62" s="71">
+        <f>AI27/AI21</f>
         <v>4.011038120819291E-3</v>
       </c>
-      <c r="AO65">
-        <f t="shared" si="46"/>
+      <c r="BO62" s="82">
+        <f>AI21/AI27</f>
         <v>249.31201596152891</v>
       </c>
-      <c r="AQ65">
-        <f t="shared" si="47"/>
+      <c r="BP62" s="83">
+        <f>AI15/AI27</f>
         <v>412.72866025335713</v>
       </c>
-      <c r="AS65">
-        <f t="shared" si="48"/>
+      <c r="BQ62" s="82">
+        <f>AI9/AI27</f>
         <v>1860.7376165331611</v>
       </c>
     </row>
-    <row r="66" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI66" t="s">
+    <row r="63" spans="48:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AV63" s="58"/>
+      <c r="AW63" s="58"/>
+      <c r="AX63" s="58"/>
+      <c r="AY63" s="58"/>
+      <c r="BL63" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM63" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN63" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="AK66" t="s">
+      <c r="BO63" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="AM66" t="s">
+      <c r="BP63" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="AO66" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ66" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS66" t="s">
+      <c r="BQ63" s="79" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI67">
+    <row r="64" spans="48:69" x14ac:dyDescent="0.35">
+      <c r="BL64" s="81">
         <f>$AI$34/AI22</f>
         <v>0.27859413510681263</v>
       </c>
-      <c r="AK67">
+      <c r="BM64" s="82">
         <f>AI28/AI22</f>
         <v>0.13658284205534707</v>
       </c>
-      <c r="AM67" s="30">
+      <c r="BN64" s="87">
         <f>AI22/AI28</f>
         <v>7.3215638578876021</v>
       </c>
-      <c r="AO67">
+      <c r="BO64" s="82">
         <f>AI16/AI28</f>
         <v>150.39671347667448</v>
       </c>
-      <c r="AQ67">
+      <c r="BP64" s="83">
         <f>AI10/AI28</f>
         <v>233.26329691761191</v>
       </c>
-      <c r="AS67">
+      <c r="BQ64" s="82">
         <f>AI4/AI28</f>
         <v>1032.5936798452644</v>
       </c>
     </row>
-    <row r="68" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI68">
+    <row r="65" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL65" s="81">
         <f>$AI$35/AI23</f>
         <v>0.32733880826659006</v>
       </c>
-      <c r="AK68">
-        <f t="shared" ref="AK68:AK72" si="49">AI29/AI23</f>
+      <c r="BM65" s="82">
+        <f>AI29/AI23</f>
         <v>0.15996116367061375</v>
       </c>
-      <c r="AM68" s="30">
-        <f t="shared" ref="AM68:AM72" si="50">AI23/AI29</f>
+      <c r="BN65" s="87">
+        <f>AI23/AI29</f>
         <v>6.2515174124337074</v>
       </c>
-      <c r="AO68">
-        <f t="shared" ref="AO68:AO72" si="51">AI17/AI29</f>
+      <c r="BO65" s="82">
+        <f>AI17/AI29</f>
         <v>279.01616976870798</v>
       </c>
-      <c r="AQ68">
-        <f t="shared" ref="AQ68:AQ72" si="52">AI11/AI29</f>
+      <c r="BP65" s="83">
+        <f>AI11/AI29</f>
         <v>436.75746355185407</v>
       </c>
-      <c r="AS68">
-        <f t="shared" ref="AS68:AS72" si="53">AI5/AI29</f>
+      <c r="BQ65" s="82">
+        <f>AI5/AI29</f>
         <v>2066.4136007541692</v>
       </c>
     </row>
-    <row r="69" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI69">
+    <row r="66" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL66" s="81">
         <f>$AI$36/AI24</f>
         <v>0.34997252159128145</v>
       </c>
-      <c r="AK69">
-        <f t="shared" si="49"/>
+      <c r="BM66" s="82">
+        <f>AI30/AI24</f>
         <v>0.16649278326461553</v>
       </c>
-      <c r="AM69" s="30">
-        <f t="shared" si="50"/>
+      <c r="BN66" s="87">
+        <f>AI24/AI30</f>
         <v>6.0062663401491019</v>
       </c>
-      <c r="AO69">
-        <f t="shared" si="51"/>
+      <c r="BO66" s="82">
+        <f>AI18/AI30</f>
         <v>490.1429984244956</v>
       </c>
-      <c r="AQ69">
-        <f t="shared" si="52"/>
+      <c r="BP66" s="83">
+        <f>AI12/AI30</f>
         <v>778.3972696966581</v>
       </c>
-      <c r="AS69">
-        <f t="shared" si="53"/>
+      <c r="BQ66" s="82">
+        <f>AI6/AI30</f>
         <v>3528.0602830199446</v>
       </c>
     </row>
-    <row r="70" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI70">
+    <row r="67" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL67" s="81">
         <f>$AI$37/AI25</f>
         <v>0.3839034071056035</v>
       </c>
-      <c r="AK70">
-        <f t="shared" si="49"/>
+      <c r="BM67" s="82">
+        <f>AI31/AI25</f>
         <v>0.17138671361228405</v>
       </c>
-      <c r="AM70" s="30">
-        <f t="shared" si="50"/>
+      <c r="BN67" s="87">
+        <f>AI25/AI31</f>
         <v>5.8347580096682909</v>
       </c>
-      <c r="AO70">
-        <f t="shared" si="51"/>
+      <c r="BO67" s="82">
+        <f>AI19/AI31</f>
         <v>802.94688339925847</v>
       </c>
-      <c r="AQ70">
-        <f t="shared" si="52"/>
+      <c r="BP67" s="83">
+        <f>AI13/AI31</f>
         <v>1256.8905137366121</v>
       </c>
-      <c r="AS70">
-        <f t="shared" si="53"/>
+      <c r="BQ67" s="82">
+        <f>AI7/AI31</f>
         <v>6013.4195221985592</v>
       </c>
     </row>
-    <row r="71" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI71">
+    <row r="68" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL68" s="81">
         <f>$AI$38/AI26</f>
         <v>0.3923716891197348</v>
       </c>
-      <c r="AK71">
-        <f t="shared" si="49"/>
+      <c r="BM68" s="82">
+        <f>AI32/AI26</f>
         <v>0.17669534752219559</v>
       </c>
-      <c r="AM71" s="30">
-        <f t="shared" si="50"/>
+      <c r="BN68" s="87">
+        <f>AI26/AI32</f>
         <v>5.6594585767142789</v>
       </c>
-      <c r="AO71">
-        <f t="shared" si="51"/>
+      <c r="BO68" s="82">
+        <f>AI20/AI32</f>
         <v>1108.5557360923015</v>
       </c>
-      <c r="AQ71">
-        <f t="shared" si="52"/>
+      <c r="BP68" s="83">
+        <f>AI14/AI32</f>
         <v>1833.8620422499973</v>
       </c>
-      <c r="AS71">
-        <f t="shared" si="53"/>
+      <c r="BQ68" s="82">
+        <f>AI8/AI32</f>
         <v>8458.8542254671192</v>
       </c>
     </row>
-    <row r="72" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI72">
+    <row r="69" spans="64:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL69" s="81">
         <f>$AI$39/AI27</f>
         <v>0.40994485520777529</v>
       </c>
-      <c r="AK72">
-        <f t="shared" si="49"/>
+      <c r="BM69" s="82">
+        <f>AI33/AI27</f>
         <v>0.17989151895950645</v>
       </c>
-      <c r="AM72" s="30">
-        <f t="shared" si="50"/>
+      <c r="BN69" s="87">
+        <f>AI27/AI33</f>
         <v>5.5589057548905334</v>
       </c>
-      <c r="AO72">
-        <f t="shared" si="51"/>
+      <c r="BO69" s="82">
+        <f>AI21/AI33</f>
         <v>1385.9020002919037</v>
       </c>
-      <c r="AQ72">
-        <f t="shared" si="52"/>
+      <c r="BP69" s="83">
+        <f>AI15/AI33</f>
         <v>2294.319724690647</v>
       </c>
-      <c r="AS72">
-        <f t="shared" si="53"/>
+      <c r="BQ69" s="82">
+        <f>AI9/AI33</f>
         <v>10343.665044887484</v>
       </c>
     </row>
-    <row r="73" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI73" t="s">
+    <row r="70" spans="64:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL70" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="BM70" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN70" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="AK73" t="s">
+      <c r="BO70" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="AM73" t="s">
+      <c r="BP70" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="AO73" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ73" t="s">
-        <v>74</v>
-      </c>
-      <c r="AS73" t="s">
+      <c r="BQ70" s="79" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI74" s="30">
+    <row r="71" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL71" s="88">
         <f>$AI$34/AI28</f>
         <v>2.0397447506174951</v>
       </c>
-      <c r="AK74">
+      <c r="BM71" s="82">
         <f>AI28/AI34</f>
         <v>0.4902574205411086</v>
       </c>
-      <c r="AM74">
+      <c r="BN71" s="83">
         <f>AI22/AI34</f>
         <v>3.5894510112949836</v>
       </c>
-      <c r="AO74">
+      <c r="BO71" s="82">
         <f>AI16/AI34</f>
         <v>73.733104806934605</v>
       </c>
-      <c r="AQ74" s="32">
+      <c r="BP71" s="89">
         <f>AI10/AI34</f>
         <v>114.35906225374313</v>
       </c>
-      <c r="AS74">
+      <c r="BQ71" s="82">
         <f>AI4/AI34</f>
         <v>506.23671394799061</v>
       </c>
     </row>
-    <row r="75" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI75" s="30">
+    <row r="72" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL72" s="88">
         <f>$AI$35/AI29</f>
         <v>2.0463642596438865</v>
       </c>
-      <c r="AK75">
-        <f t="shared" ref="AK75:AK79" si="54">AI29/AI35</f>
+      <c r="BM72" s="82">
+        <f>AI29/AI35</f>
         <v>0.48867155262671685</v>
       </c>
-      <c r="AM75">
-        <f t="shared" ref="AM75:AM79" si="55">AI23/AI35</f>
+      <c r="BN72" s="83">
+        <f>AI23/AI35</f>
         <v>3.0549387202069354</v>
       </c>
-      <c r="AO75">
-        <f t="shared" ref="AO75:AO79" si="56">AI17/AI35</f>
+      <c r="BO72" s="82">
+        <f>AI17/AI35</f>
         <v>136.34726488883416</v>
       </c>
-      <c r="AQ75">
-        <f t="shared" ref="AQ75:AQ79" si="57">AI11/AI35</f>
+      <c r="BP72" s="83">
+        <f>AI11/AI35</f>
         <v>213.43094783519123</v>
       </c>
-      <c r="AS75">
-        <f t="shared" ref="AS75:AS79" si="58">AI5/AI35</f>
+      <c r="BQ72" s="82">
+        <f>AI5/AI35</f>
         <v>1009.7975426495044</v>
       </c>
     </row>
-    <row r="76" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI76" s="30">
+    <row r="73" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL73" s="88">
         <f>$AI$36/AI30</f>
         <v>2.1020281764108186</v>
       </c>
-      <c r="AK76">
-        <f t="shared" si="54"/>
+      <c r="BM73" s="82">
+        <f>AI30/AI36</f>
         <v>0.47573101598832274</v>
       </c>
-      <c r="AM76">
-        <f t="shared" si="55"/>
+      <c r="BN73" s="83">
+        <f>AI24/AI36</f>
         <v>2.8573671882955969</v>
       </c>
-      <c r="AO76">
-        <f t="shared" si="56"/>
+      <c r="BO73" s="82">
+        <f>AI18/AI36</f>
         <v>233.17622662004817</v>
       </c>
-      <c r="AQ76">
-        <f t="shared" si="57"/>
+      <c r="BP73" s="83">
+        <f>AI12/AI36</f>
         <v>370.30772395532762</v>
       </c>
-      <c r="AS76">
-        <f t="shared" si="58"/>
+      <c r="BQ73" s="82">
+        <f>AI6/AI36</f>
         <v>1678.4077029091275</v>
       </c>
     </row>
-    <row r="77" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI77" s="30">
+    <row r="74" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL74" s="88">
         <f>$AI$37/AI31</f>
         <v>2.2399834795483669</v>
       </c>
-      <c r="AK77">
-        <f t="shared" si="54"/>
+      <c r="BM74" s="82">
+        <f>AI31/AI37</f>
         <v>0.44643186395357853</v>
       </c>
-      <c r="AM77">
-        <f t="shared" si="55"/>
+      <c r="BN74" s="83">
+        <f>AI25/AI37</f>
         <v>2.6048218939742873</v>
       </c>
-      <c r="AO77">
-        <f t="shared" si="56"/>
+      <c r="BO74" s="82">
+        <f>AI19/AI37</f>
         <v>358.46107381164762</v>
       </c>
-      <c r="AQ77">
-        <f t="shared" si="57"/>
+      <c r="BP74" s="83">
+        <f>AI13/AI37</f>
         <v>561.1159748330067</v>
       </c>
-      <c r="AS77">
-        <f t="shared" si="58"/>
+      <c r="BQ74" s="82">
+        <f>AI7/AI37</f>
         <v>2684.5820860299405</v>
       </c>
     </row>
-    <row r="78" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI78" s="30">
+    <row r="75" spans="64:69" x14ac:dyDescent="0.35">
+      <c r="BL75" s="88">
         <f>$AI$38/AI32</f>
         <v>2.2206113212485517</v>
       </c>
-      <c r="AK78">
-        <f t="shared" si="54"/>
+      <c r="BM75" s="82">
+        <f>AI32/AI38</f>
         <v>0.45032644408826311</v>
       </c>
-      <c r="AM78">
-        <f t="shared" si="55"/>
+      <c r="BN75" s="83">
+        <f>AI26/AI38</f>
         <v>2.5486038563165638</v>
       </c>
-      <c r="AO78">
-        <f t="shared" si="56"/>
+      <c r="BO75" s="82">
+        <f>AI20/AI38</f>
         <v>499.21196270809315</v>
       </c>
-      <c r="AQ78">
-        <f t="shared" si="57"/>
+      <c r="BP75" s="83">
+        <f>AI14/AI38</f>
         <v>825.83657243488142</v>
       </c>
-      <c r="AS78">
-        <f t="shared" si="58"/>
+      <c r="BQ75" s="82">
+        <f>AI8/AI38</f>
         <v>3809.2457444155866</v>
       </c>
     </row>
-    <row r="79" spans="35:45" x14ac:dyDescent="0.35">
-      <c r="AI79" s="30">
+    <row r="76" spans="64:69" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BL76" s="90">
         <f>$AI$39/AI33</f>
         <v>2.2788448148022686</v>
       </c>
-      <c r="AK79">
-        <f t="shared" si="54"/>
+      <c r="BM76" s="91">
+        <f>AI33/AI39</f>
         <v>0.43881882324960692</v>
       </c>
-      <c r="AM79">
-        <f t="shared" si="55"/>
+      <c r="BN76" s="92">
+        <f>AI27/AI39</f>
         <v>2.439352481916532</v>
       </c>
-      <c r="AO79">
-        <f t="shared" si="56"/>
+      <c r="BO76" s="91">
+        <f>AI21/AI39</f>
         <v>608.15988490736959</v>
       </c>
-      <c r="AQ79">
-        <f t="shared" si="57"/>
+      <c r="BP76" s="92">
+        <f>AI15/AI39</f>
         <v>1006.7906817471119</v>
       </c>
-      <c r="AS79">
-        <f t="shared" si="58"/>
+      <c r="BQ76" s="91">
+        <f>AI9/AI39</f>
         <v>4538.9949230856182</v>
       </c>
     </row>
     <row r="85" spans="41:41" x14ac:dyDescent="0.35">
       <c r="AO85" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO86" s="31">
+      <c r="AO86" s="30">
         <f>AO34/LOG(C34, 2)</f>
         <v>7.0631991928678879E-5</v>
       </c>
     </row>
     <row r="87" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO87" s="31">
-        <f t="shared" ref="AO87:AO91" si="59">AO35/LOG(C35, 2)</f>
+      <c r="AO87" s="30">
+        <f>AO35/LOG(C35, 2)</f>
         <v>1.377693878155776E-4</v>
       </c>
     </row>
     <row r="88" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO88" s="31">
-        <f t="shared" si="59"/>
+      <c r="AO88" s="30">
+        <f>AO36/LOG(C36, 2)</f>
         <v>2.3395654113913096E-4</v>
       </c>
     </row>
     <row r="89" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO89" s="31">
-        <f t="shared" si="59"/>
+      <c r="AO89" s="30">
+        <f>AO37/LOG(C37, 2)</f>
         <v>3.9732991205526619E-4</v>
       </c>
     </row>
     <row r="90" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO90" s="31">
-        <f t="shared" si="59"/>
+      <c r="AO90" s="30">
+        <f>AO38/LOG(C38, 2)</f>
         <v>5.4442657924767943E-4</v>
       </c>
     </row>
     <row r="91" spans="41:41" x14ac:dyDescent="0.35">
-      <c r="AO91" s="31">
-        <f t="shared" si="59"/>
+      <c r="AO91" s="30">
+        <f>AO39/LOG(C39, 2)</f>
         <v>7.266509839790635E-4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="BE27:BF32"/>
-    <mergeCell ref="BA33:BB38"/>
-    <mergeCell ref="BC33:BD38"/>
-    <mergeCell ref="BE33:BF38"/>
-    <mergeCell ref="BE3:BF8"/>
-    <mergeCell ref="BC9:BD14"/>
-    <mergeCell ref="BE9:BF14"/>
-    <mergeCell ref="BC15:BD20"/>
-    <mergeCell ref="BE15:BF20"/>
-    <mergeCell ref="BC21:BD26"/>
-    <mergeCell ref="BE21:BF26"/>
-    <mergeCell ref="BC27:BD32"/>
-    <mergeCell ref="BC3:BD8"/>
-    <mergeCell ref="AY33:AZ38"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="AY9:AZ14"/>
-    <mergeCell ref="AY15:AZ20"/>
-    <mergeCell ref="AY21:AZ26"/>
-    <mergeCell ref="AY27:AZ32"/>
-    <mergeCell ref="BA9:BB14"/>
-    <mergeCell ref="BA15:BB20"/>
-    <mergeCell ref="BA21:BB26"/>
-    <mergeCell ref="BA27:BB32"/>
-    <mergeCell ref="AD2:AI2"/>
-    <mergeCell ref="AJ2:AO2"/>
-    <mergeCell ref="AP2:AU2"/>
-    <mergeCell ref="AY1:BD1"/>
-    <mergeCell ref="BE1:BF2"/>
-    <mergeCell ref="AC22:AC27"/>
-    <mergeCell ref="AC28:AC33"/>
-    <mergeCell ref="AC34:AC39"/>
-    <mergeCell ref="AC4:AC9"/>
-    <mergeCell ref="AC10:AC15"/>
-    <mergeCell ref="AC16:AC21"/>
+  <mergeCells count="75">
+    <mergeCell ref="AV55:AY63"/>
+    <mergeCell ref="BL40:BQ41"/>
+    <mergeCell ref="BG3:BH8"/>
+    <mergeCell ref="BG1:BH2"/>
+    <mergeCell ref="BG33:BH38"/>
+    <mergeCell ref="BG27:BH32"/>
+    <mergeCell ref="BG21:BH26"/>
+    <mergeCell ref="BG15:BH20"/>
+    <mergeCell ref="BG9:BH14"/>
+    <mergeCell ref="AX21:AX26"/>
+    <mergeCell ref="AX27:AX32"/>
+    <mergeCell ref="AX33:AX38"/>
+    <mergeCell ref="AX3:AX8"/>
+    <mergeCell ref="AX9:AX14"/>
+    <mergeCell ref="AX15:AX20"/>
+    <mergeCell ref="AY3:AZ8"/>
+    <mergeCell ref="BA3:BB8"/>
+    <mergeCell ref="BI27:BI32"/>
+    <mergeCell ref="BI33:BI38"/>
+    <mergeCell ref="BI1:BI2"/>
+    <mergeCell ref="BI3:BI8"/>
+    <mergeCell ref="BI9:BI14"/>
+    <mergeCell ref="BI15:BI20"/>
+    <mergeCell ref="BI21:BI26"/>
     <mergeCell ref="U2:AA2"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="N2:T2"/>
@@ -21180,29 +21279,42 @@
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="B22:B27"/>
     <mergeCell ref="B28:B33"/>
-    <mergeCell ref="BI27:BI32"/>
-    <mergeCell ref="BI33:BI38"/>
-    <mergeCell ref="BI1:BI2"/>
-    <mergeCell ref="BI3:BI8"/>
-    <mergeCell ref="BI9:BI14"/>
-    <mergeCell ref="BI15:BI20"/>
-    <mergeCell ref="BI21:BI26"/>
-    <mergeCell ref="BG3:BH8"/>
-    <mergeCell ref="BG1:BH2"/>
-    <mergeCell ref="AV55:AY63"/>
-    <mergeCell ref="BG33:BH38"/>
-    <mergeCell ref="BG27:BH32"/>
-    <mergeCell ref="BG21:BH26"/>
-    <mergeCell ref="BG15:BH20"/>
-    <mergeCell ref="BG9:BH14"/>
-    <mergeCell ref="AX21:AX26"/>
-    <mergeCell ref="AX27:AX32"/>
-    <mergeCell ref="AX33:AX38"/>
-    <mergeCell ref="AX3:AX8"/>
-    <mergeCell ref="AX9:AX14"/>
-    <mergeCell ref="AX15:AX20"/>
-    <mergeCell ref="AY3:AZ8"/>
-    <mergeCell ref="BA3:BB8"/>
+    <mergeCell ref="AC22:AC27"/>
+    <mergeCell ref="AC28:AC33"/>
+    <mergeCell ref="AC34:AC39"/>
+    <mergeCell ref="AC4:AC9"/>
+    <mergeCell ref="AC10:AC15"/>
+    <mergeCell ref="AC16:AC21"/>
+    <mergeCell ref="AD2:AI2"/>
+    <mergeCell ref="AJ2:AO2"/>
+    <mergeCell ref="AP2:AU2"/>
+    <mergeCell ref="AY1:BD1"/>
+    <mergeCell ref="BE1:BF2"/>
+    <mergeCell ref="AY33:AZ38"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="AY9:AZ14"/>
+    <mergeCell ref="AY15:AZ20"/>
+    <mergeCell ref="AY21:AZ26"/>
+    <mergeCell ref="AY27:AZ32"/>
+    <mergeCell ref="BA9:BB14"/>
+    <mergeCell ref="BA15:BB20"/>
+    <mergeCell ref="BA21:BB26"/>
+    <mergeCell ref="BA27:BB32"/>
+    <mergeCell ref="BE27:BF32"/>
+    <mergeCell ref="BA33:BB38"/>
+    <mergeCell ref="BC33:BD38"/>
+    <mergeCell ref="BE33:BF38"/>
+    <mergeCell ref="BE3:BF8"/>
+    <mergeCell ref="BC9:BD14"/>
+    <mergeCell ref="BE9:BF14"/>
+    <mergeCell ref="BC15:BD20"/>
+    <mergeCell ref="BE15:BF20"/>
+    <mergeCell ref="BC21:BD26"/>
+    <mergeCell ref="BE21:BF26"/>
+    <mergeCell ref="BC27:BD32"/>
+    <mergeCell ref="BC3:BD8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>